<commit_message>
Updated Formatting on old excel file
</commit_message>
<xml_diff>
--- a/Attributes.xlsx
+++ b/Attributes.xlsx
@@ -1,28 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\Documents\Visual Studio 2019\Projects\BESM3CA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5E72FC18-5519-427F-9D85-ACBC4E5E3042}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908D9E43-F827-4039-8B1A-2D9C4362E1A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16005" yWindow="7065" windowWidth="21600" windowHeight="11385"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="92512"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="172">
   <si>
     <t>Attribute Name</t>
   </si>
@@ -523,12 +521,27 @@
   </si>
   <si>
     <t>true</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>44</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -561,17 +574,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -885,31 +897,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="22.42578125" customWidth="1"/>
-    <col min="8" max="8" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="22.453125" customWidth="1"/>
+    <col min="8" max="8" width="7.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.54296875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>164</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -921,7 +935,7 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -934,14 +948,14 @@
       <c r="K1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A2" s="6">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>87</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D2" t="s">
@@ -953,7 +967,7 @@
       <c r="F2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="5" t="s">
         <v>10</v>
       </c>
       <c r="H2" t="s">
@@ -962,26 +976,26 @@
       <c r="I2" t="s">
         <v>82</v>
       </c>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A3" s="6">
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>88</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D3" t="s">
@@ -993,7 +1007,7 @@
       <c r="F3" t="s">
         <v>9</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H3" t="s">
@@ -1002,26 +1016,26 @@
       <c r="I3" t="s">
         <v>82</v>
       </c>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A4" s="6">
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D4" t="s">
@@ -1033,7 +1047,7 @@
       <c r="F4" t="s">
         <v>15</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H4" t="s">
@@ -1042,27 +1056,27 @@
       <c r="I4" t="s">
         <v>82</v>
       </c>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="7"/>
-      <c r="S4" s="7"/>
-      <c r="T4" s="7"/>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A5" s="6">
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>129</v>
       </c>
-      <c r="C5">
-        <v>10</v>
+      <c r="C5" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -1073,7 +1087,7 @@
       <c r="F5" t="s">
         <v>15</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="5" t="s">
         <v>26</v>
       </c>
       <c r="H5" t="s">
@@ -1082,27 +1096,27 @@
       <c r="I5" t="s">
         <v>82</v>
       </c>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A6" s="6">
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>130</v>
       </c>
-      <c r="C6">
-        <v>4</v>
+      <c r="C6" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
@@ -1113,7 +1127,7 @@
       <c r="F6" t="s">
         <v>28</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="5" t="s">
         <v>26</v>
       </c>
       <c r="H6" t="s">
@@ -1122,26 +1136,26 @@
       <c r="I6" t="s">
         <v>82</v>
       </c>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="7"/>
-      <c r="T6" s="7"/>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A7" s="6">
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>89</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="6" t="s">
         <v>132</v>
       </c>
       <c r="D7" t="s">
@@ -1153,7 +1167,7 @@
       <c r="F7" t="s">
         <v>28</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="5" t="s">
         <v>149</v>
       </c>
       <c r="H7" t="s">
@@ -1162,27 +1176,27 @@
       <c r="I7" t="s">
         <v>82</v>
       </c>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
-      <c r="T7" s="7"/>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A8" s="6">
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>90</v>
       </c>
-      <c r="C8">
-        <v>2</v>
+      <c r="C8" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
@@ -1193,7 +1207,7 @@
       <c r="F8" t="s">
         <v>15</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="5" t="s">
         <v>150</v>
       </c>
       <c r="H8" t="s">
@@ -1202,26 +1216,26 @@
       <c r="I8" t="s">
         <v>82</v>
       </c>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
-      <c r="T8" s="7"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A9" s="6">
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>19</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D9" t="s">
@@ -1233,7 +1247,7 @@
       <c r="F9" t="s">
         <v>15</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="5" t="s">
         <v>22</v>
       </c>
       <c r="H9" t="s">
@@ -1242,26 +1256,26 @@
       <c r="I9" t="s">
         <v>82</v>
       </c>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7"/>
-      <c r="S9" s="7"/>
-      <c r="T9" s="7"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A10" s="6">
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>91</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D10" t="s">
@@ -1273,7 +1287,7 @@
       <c r="F10" t="s">
         <v>24</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H10" t="s">
@@ -1282,26 +1296,26 @@
       <c r="I10" t="s">
         <v>82</v>
       </c>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="7"/>
-      <c r="S10" s="7"/>
-      <c r="T10" s="7"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A11" s="6">
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>92</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="5" t="s">
         <v>133</v>
       </c>
       <c r="D11" t="s">
@@ -1313,7 +1327,7 @@
       <c r="F11" t="s">
         <v>9</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H11" t="s">
@@ -1322,26 +1336,26 @@
       <c r="I11" t="s">
         <v>82</v>
       </c>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="7"/>
-      <c r="R11" s="7"/>
-      <c r="S11" s="7"/>
-      <c r="T11" s="7"/>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A12" s="6">
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>93</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="6" t="s">
         <v>134</v>
       </c>
       <c r="D12" t="s">
@@ -1353,7 +1367,7 @@
       <c r="F12" t="s">
         <v>9</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H12" t="s">
@@ -1362,27 +1376,27 @@
       <c r="I12" t="s">
         <v>82</v>
       </c>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="7"/>
-      <c r="S12" s="7"/>
-      <c r="T12" s="7"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A13" s="6">
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
         <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>131</v>
       </c>
-      <c r="C13">
-        <v>10</v>
+      <c r="C13" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>
@@ -1393,7 +1407,7 @@
       <c r="F13" t="s">
         <v>15</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="5" t="s">
         <v>29</v>
       </c>
       <c r="H13" t="s">
@@ -1402,26 +1416,26 @@
       <c r="I13" t="s">
         <v>82</v>
       </c>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="7"/>
-      <c r="R13" s="7"/>
-      <c r="S13" s="7"/>
-      <c r="T13" s="7"/>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A14" s="6">
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
         <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>94</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="5" t="s">
         <v>27</v>
       </c>
       <c r="D14" t="s">
@@ -1433,7 +1447,7 @@
       <c r="F14" t="s">
         <v>28</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="5" t="s">
         <v>29</v>
       </c>
       <c r="H14" t="s">
@@ -1442,26 +1456,26 @@
       <c r="I14" t="s">
         <v>82</v>
       </c>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
-      <c r="P14" s="7"/>
-      <c r="Q14" s="7"/>
-      <c r="R14" s="7"/>
-      <c r="S14" s="7"/>
-      <c r="T14" s="7"/>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A15" s="6">
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
         <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>95</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D15" t="s">
@@ -1473,7 +1487,7 @@
       <c r="F15" t="s">
         <v>28</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="5" t="s">
         <v>151</v>
       </c>
       <c r="H15" t="s">
@@ -1482,27 +1496,27 @@
       <c r="I15" t="s">
         <v>82</v>
       </c>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="7"/>
-      <c r="S15" s="7"/>
-      <c r="T15" s="7"/>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A16" s="6">
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
+      <c r="T15" s="3"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
         <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>96</v>
       </c>
-      <c r="C16">
-        <v>2</v>
+      <c r="C16" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D16" t="s">
         <v>7</v>
@@ -1513,7 +1527,7 @@
       <c r="F16" t="s">
         <v>15</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="5" t="s">
         <v>33</v>
       </c>
       <c r="H16" t="s">
@@ -1522,26 +1536,26 @@
       <c r="I16" t="s">
         <v>82</v>
       </c>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="7"/>
-      <c r="Q16" s="7"/>
-      <c r="R16" s="7"/>
-      <c r="S16" s="7"/>
-      <c r="T16" s="7"/>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A17" s="6">
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="3"/>
+      <c r="T16" s="3"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
         <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>97</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="5" t="s">
         <v>135</v>
       </c>
       <c r="D17" t="s">
@@ -1553,7 +1567,7 @@
       <c r="F17" t="s">
         <v>57</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="5" t="s">
         <v>33</v>
       </c>
       <c r="H17" t="s">
@@ -1562,26 +1576,26 @@
       <c r="I17" t="s">
         <v>82</v>
       </c>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="7"/>
-      <c r="P17" s="7"/>
-      <c r="Q17" s="7"/>
-      <c r="R17" s="7"/>
-      <c r="S17" s="7"/>
-      <c r="T17" s="7"/>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A18" s="6">
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="3"/>
+      <c r="T17" s="3"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
         <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>31</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D18" t="s">
@@ -1593,7 +1607,7 @@
       <c r="F18" t="s">
         <v>9</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" s="5" t="s">
         <v>33</v>
       </c>
       <c r="H18" t="s">
@@ -1602,27 +1616,27 @@
       <c r="I18" t="s">
         <v>82</v>
       </c>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="7"/>
-      <c r="Q18" s="7"/>
-      <c r="R18" s="7"/>
-      <c r="S18" s="7"/>
-      <c r="T18" s="7"/>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A19" s="6">
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3"/>
+      <c r="S18" s="3"/>
+      <c r="T18" s="3"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
         <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>98</v>
       </c>
-      <c r="C19">
-        <v>2</v>
+      <c r="C19" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D19" t="s">
         <v>7</v>
@@ -1633,7 +1647,7 @@
       <c r="F19" t="s">
         <v>15</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="5" t="s">
         <v>30</v>
       </c>
       <c r="H19" t="s">
@@ -1642,27 +1656,27 @@
       <c r="I19" t="s">
         <v>82</v>
       </c>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
-      <c r="O19" s="7"/>
-      <c r="P19" s="7"/>
-      <c r="Q19" s="7"/>
-      <c r="R19" s="7"/>
-      <c r="S19" s="7"/>
-      <c r="T19" s="7"/>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A20" s="6">
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+      <c r="S19" s="3"/>
+      <c r="T19" s="3"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
         <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>99</v>
       </c>
-      <c r="C20">
-        <v>10</v>
+      <c r="C20" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="D20" t="s">
         <v>7</v>
@@ -1673,7 +1687,7 @@
       <c r="F20" t="s">
         <v>15</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20" s="5" t="s">
         <v>30</v>
       </c>
       <c r="H20" t="s">
@@ -1682,26 +1696,26 @@
       <c r="I20" t="s">
         <v>82</v>
       </c>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
-      <c r="O20" s="7"/>
-      <c r="P20" s="7"/>
-      <c r="Q20" s="7"/>
-      <c r="R20" s="7"/>
-      <c r="S20" s="7"/>
-      <c r="T20" s="7"/>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A21" s="6">
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="3"/>
+      <c r="T20" s="3"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
         <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>100</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D21" t="s">
@@ -1713,7 +1727,7 @@
       <c r="F21" t="s">
         <v>28</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="5" t="s">
         <v>30</v>
       </c>
       <c r="H21" t="s">
@@ -1722,26 +1736,26 @@
       <c r="I21" t="s">
         <v>82</v>
       </c>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="7"/>
-      <c r="P21" s="7"/>
-      <c r="Q21" s="7"/>
-      <c r="R21" s="7"/>
-      <c r="S21" s="7"/>
-      <c r="T21" s="7"/>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A22" s="6">
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3"/>
+      <c r="T21" s="3"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
         <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>34</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D22" t="s">
@@ -1753,7 +1767,7 @@
       <c r="F22" t="s">
         <v>28</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="5" t="s">
         <v>30</v>
       </c>
       <c r="H22" t="s">
@@ -1762,26 +1776,26 @@
       <c r="I22" t="s">
         <v>82</v>
       </c>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7"/>
-      <c r="O22" s="7"/>
-      <c r="P22" s="7"/>
-      <c r="Q22" s="7"/>
-      <c r="R22" s="7"/>
-      <c r="S22" s="7"/>
-      <c r="T22" s="7"/>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A23" s="6">
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="3"/>
+      <c r="T22" s="3"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
         <v>22</v>
       </c>
       <c r="B23" t="s">
         <v>101</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D23" t="s">
@@ -1793,7 +1807,7 @@
       <c r="F23" t="s">
         <v>15</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23" s="5" t="s">
         <v>35</v>
       </c>
       <c r="H23" t="s">
@@ -1802,27 +1816,27 @@
       <c r="I23" t="s">
         <v>82</v>
       </c>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
-      <c r="L23" s="7"/>
-      <c r="M23" s="7"/>
-      <c r="N23" s="7"/>
-      <c r="O23" s="7"/>
-      <c r="P23" s="7"/>
-      <c r="Q23" s="7"/>
-      <c r="R23" s="7"/>
-      <c r="S23" s="7"/>
-      <c r="T23" s="7"/>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A24" s="6">
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="3"/>
+      <c r="T23" s="3"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
         <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>102</v>
       </c>
-      <c r="C24">
-        <v>15</v>
+      <c r="C24" s="5" t="s">
+        <v>167</v>
       </c>
       <c r="D24" t="s">
         <v>7</v>
@@ -1833,7 +1847,7 @@
       <c r="F24" t="s">
         <v>15</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" s="5" t="s">
         <v>35</v>
       </c>
       <c r="H24" t="s">
@@ -1842,27 +1856,27 @@
       <c r="I24" t="s">
         <v>82</v>
       </c>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
-      <c r="M24" s="7"/>
-      <c r="N24" s="7"/>
-      <c r="O24" s="7"/>
-      <c r="P24" s="7"/>
-      <c r="Q24" s="7"/>
-      <c r="R24" s="7"/>
-      <c r="S24" s="7"/>
-      <c r="T24" s="7"/>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A25" s="6">
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
+      <c r="S24" s="3"/>
+      <c r="T24" s="3"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
         <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>103</v>
       </c>
-      <c r="C25">
-        <v>5</v>
+      <c r="C25" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="D25" t="s">
         <v>7</v>
@@ -1873,7 +1887,7 @@
       <c r="F25" t="s">
         <v>15</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G25" s="5" t="s">
         <v>35</v>
       </c>
       <c r="H25" t="s">
@@ -1882,26 +1896,26 @@
       <c r="I25" t="s">
         <v>82</v>
       </c>
-      <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
-      <c r="L25" s="7"/>
-      <c r="M25" s="7"/>
-      <c r="N25" s="7"/>
-      <c r="O25" s="7"/>
-      <c r="P25" s="7"/>
-      <c r="Q25" s="7"/>
-      <c r="R25" s="7"/>
-      <c r="S25" s="7"/>
-      <c r="T25" s="7"/>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A26" s="6">
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+      <c r="S25" s="3"/>
+      <c r="T25" s="3"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
         <v>25</v>
       </c>
       <c r="B26" t="s">
         <v>37</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="5" t="s">
         <v>38</v>
       </c>
       <c r="D26" t="s">
@@ -1913,7 +1927,7 @@
       <c r="F26" t="s">
         <v>15</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G26" s="5" t="s">
         <v>35</v>
       </c>
       <c r="H26" t="s">
@@ -1922,26 +1936,26 @@
       <c r="I26" t="s">
         <v>82</v>
       </c>
-      <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="7"/>
-      <c r="M26" s="7"/>
-      <c r="N26" s="7"/>
-      <c r="O26" s="7"/>
-      <c r="P26" s="7"/>
-      <c r="Q26" s="7"/>
-      <c r="R26" s="7"/>
-      <c r="S26" s="7"/>
-      <c r="T26" s="7"/>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A27" s="6">
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="3"/>
+      <c r="S26" s="3"/>
+      <c r="T26" s="3"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
         <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>39</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="5" t="s">
         <v>27</v>
       </c>
       <c r="D27" t="s">
@@ -1953,7 +1967,7 @@
       <c r="F27" t="s">
         <v>9</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G27" s="5" t="s">
         <v>41</v>
       </c>
       <c r="H27" t="s">
@@ -1962,26 +1976,26 @@
       <c r="I27" t="s">
         <v>82</v>
       </c>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="7"/>
-      <c r="M27" s="7"/>
-      <c r="N27" s="7"/>
-      <c r="O27" s="7"/>
-      <c r="P27" s="7"/>
-      <c r="Q27" s="7"/>
-      <c r="R27" s="7"/>
-      <c r="S27" s="7"/>
-      <c r="T27" s="7"/>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A28" s="6">
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="3"/>
+      <c r="S27" s="3"/>
+      <c r="T27" s="3"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
         <v>27</v>
       </c>
       <c r="B28" t="s">
         <v>104</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="5" t="s">
         <v>42</v>
       </c>
       <c r="D28" t="s">
@@ -1993,7 +2007,7 @@
       <c r="F28" t="s">
         <v>24</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G28" s="5" t="s">
         <v>43</v>
       </c>
       <c r="H28" t="s">
@@ -2002,26 +2016,26 @@
       <c r="I28" t="s">
         <v>82</v>
       </c>
-      <c r="J28" s="7"/>
-      <c r="K28" s="7"/>
-      <c r="L28" s="7"/>
-      <c r="M28" s="7"/>
-      <c r="N28" s="7"/>
-      <c r="O28" s="7"/>
-      <c r="P28" s="7"/>
-      <c r="Q28" s="7"/>
-      <c r="R28" s="7"/>
-      <c r="S28" s="7"/>
-      <c r="T28" s="7"/>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A29" s="6">
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="3"/>
+      <c r="R28" s="3"/>
+      <c r="S28" s="3"/>
+      <c r="T28" s="3"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
         <v>28</v>
       </c>
       <c r="B29" t="s">
         <v>44</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D29" t="s">
@@ -2033,8 +2047,8 @@
       <c r="F29" t="s">
         <v>153</v>
       </c>
-      <c r="G29">
-        <v>35</v>
+      <c r="G29" s="5" t="s">
+        <v>168</v>
       </c>
       <c r="H29" t="s">
         <v>165</v>
@@ -2042,27 +2056,27 @@
       <c r="I29" t="s">
         <v>82</v>
       </c>
-      <c r="J29" s="7"/>
-      <c r="K29" s="7"/>
-      <c r="L29" s="7"/>
-      <c r="M29" s="7"/>
-      <c r="N29" s="7"/>
-      <c r="O29" s="7"/>
-      <c r="P29" s="7"/>
-      <c r="Q29" s="7"/>
-      <c r="R29" s="7"/>
-      <c r="S29" s="7"/>
-      <c r="T29" s="7"/>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A30" s="6">
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
+      <c r="R29" s="3"/>
+      <c r="S29" s="3"/>
+      <c r="T29" s="3"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
         <v>29</v>
       </c>
       <c r="B30" t="s">
         <v>105</v>
       </c>
-      <c r="C30">
-        <v>2</v>
+      <c r="C30" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D30" t="s">
         <v>7</v>
@@ -2073,8 +2087,8 @@
       <c r="F30" t="s">
         <v>154</v>
       </c>
-      <c r="G30">
-        <v>35</v>
+      <c r="G30" s="5" t="s">
+        <v>168</v>
       </c>
       <c r="H30" t="s">
         <v>166</v>
@@ -2082,27 +2096,27 @@
       <c r="I30" t="s">
         <v>82</v>
       </c>
-      <c r="J30" s="7"/>
-      <c r="K30" s="7"/>
-      <c r="L30" s="7"/>
-      <c r="M30" s="7"/>
-      <c r="N30" s="7"/>
-      <c r="O30" s="7"/>
-      <c r="P30" s="7"/>
-      <c r="Q30" s="7"/>
-      <c r="R30" s="7"/>
-      <c r="S30" s="7"/>
-      <c r="T30" s="7"/>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A31" s="6">
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+      <c r="P30" s="3"/>
+      <c r="Q30" s="3"/>
+      <c r="R30" s="3"/>
+      <c r="S30" s="3"/>
+      <c r="T30" s="3"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
         <v>30</v>
       </c>
       <c r="B31" t="s">
         <v>106</v>
       </c>
-      <c r="C31">
-        <v>2</v>
+      <c r="C31" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D31" t="s">
         <v>7</v>
@@ -2113,8 +2127,8 @@
       <c r="F31" t="s">
         <v>154</v>
       </c>
-      <c r="G31">
-        <v>35</v>
+      <c r="G31" s="5" t="s">
+        <v>168</v>
       </c>
       <c r="H31" t="s">
         <v>166</v>
@@ -2122,26 +2136,26 @@
       <c r="I31" t="s">
         <v>82</v>
       </c>
-      <c r="J31" s="7"/>
-      <c r="K31" s="7"/>
-      <c r="L31" s="7"/>
-      <c r="M31" s="7"/>
-      <c r="N31" s="7"/>
-      <c r="O31" s="7"/>
-      <c r="P31" s="7"/>
-      <c r="Q31" s="7"/>
-      <c r="R31" s="7"/>
-      <c r="S31" s="7"/>
-      <c r="T31" s="7"/>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A32" s="6">
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
+      <c r="P31" s="3"/>
+      <c r="Q31" s="3"/>
+      <c r="R31" s="3"/>
+      <c r="S31" s="3"/>
+      <c r="T31" s="3"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
         <v>31</v>
       </c>
       <c r="B32" t="s">
         <v>45</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D32" t="s">
@@ -2153,7 +2167,7 @@
       <c r="F32" t="s">
         <v>24</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G32" s="5" t="s">
         <v>46</v>
       </c>
       <c r="H32" t="s">
@@ -2162,26 +2176,26 @@
       <c r="I32" t="s">
         <v>82</v>
       </c>
-      <c r="J32" s="7"/>
-      <c r="K32" s="7"/>
-      <c r="L32" s="7"/>
-      <c r="M32" s="7"/>
-      <c r="N32" s="7"/>
-      <c r="O32" s="7"/>
-      <c r="P32" s="7"/>
-      <c r="Q32" s="7"/>
-      <c r="R32" s="7"/>
-      <c r="S32" s="7"/>
-      <c r="T32" s="7"/>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A33" s="6">
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+      <c r="P32" s="3"/>
+      <c r="Q32" s="3"/>
+      <c r="R32" s="3"/>
+      <c r="S32" s="3"/>
+      <c r="T32" s="3"/>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
         <v>32</v>
       </c>
       <c r="B33" t="s">
         <v>47</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="5" t="s">
         <v>27</v>
       </c>
       <c r="D33" t="s">
@@ -2193,7 +2207,7 @@
       <c r="F33" t="s">
         <v>9</v>
       </c>
-      <c r="G33" t="s">
+      <c r="G33" s="5" t="s">
         <v>46</v>
       </c>
       <c r="H33" t="s">
@@ -2202,26 +2216,26 @@
       <c r="I33" t="s">
         <v>82</v>
       </c>
-      <c r="J33" s="7"/>
-      <c r="K33" s="7"/>
-      <c r="L33" s="7"/>
-      <c r="M33" s="7"/>
-      <c r="N33" s="7"/>
-      <c r="O33" s="7"/>
-      <c r="P33" s="7"/>
-      <c r="Q33" s="7"/>
-      <c r="R33" s="7"/>
-      <c r="S33" s="7"/>
-      <c r="T33" s="7"/>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A34" s="6">
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
+      <c r="P33" s="3"/>
+      <c r="Q33" s="3"/>
+      <c r="R33" s="3"/>
+      <c r="S33" s="3"/>
+      <c r="T33" s="3"/>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
         <v>33</v>
       </c>
       <c r="B34" t="s">
         <v>48</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D34" t="s">
@@ -2233,7 +2247,7 @@
       <c r="F34" t="s">
         <v>9</v>
       </c>
-      <c r="G34" t="s">
+      <c r="G34" s="5" t="s">
         <v>49</v>
       </c>
       <c r="H34" t="s">
@@ -2242,26 +2256,26 @@
       <c r="I34" t="s">
         <v>82</v>
       </c>
-      <c r="J34" s="7"/>
-      <c r="K34" s="7"/>
-      <c r="L34" s="7"/>
-      <c r="M34" s="7"/>
-      <c r="N34" s="7"/>
-      <c r="O34" s="7"/>
-      <c r="P34" s="7"/>
-      <c r="Q34" s="7"/>
-      <c r="R34" s="7"/>
-      <c r="S34" s="7"/>
-      <c r="T34" s="7"/>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A35" s="6">
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
+      <c r="O34" s="3"/>
+      <c r="P34" s="3"/>
+      <c r="Q34" s="3"/>
+      <c r="R34" s="3"/>
+      <c r="S34" s="3"/>
+      <c r="T34" s="3"/>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
         <v>34</v>
       </c>
       <c r="B35" t="s">
         <v>50</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D35" t="s">
@@ -2273,7 +2287,7 @@
       <c r="F35" t="s">
         <v>15</v>
       </c>
-      <c r="G35" t="s">
+      <c r="G35" s="5" t="s">
         <v>49</v>
       </c>
       <c r="H35" t="s">
@@ -2282,26 +2296,26 @@
       <c r="I35" t="s">
         <v>82</v>
       </c>
-      <c r="J35" s="7"/>
-      <c r="K35" s="7"/>
-      <c r="L35" s="7"/>
-      <c r="M35" s="7"/>
-      <c r="N35" s="7"/>
-      <c r="O35" s="7"/>
-      <c r="P35" s="7"/>
-      <c r="Q35" s="7"/>
-      <c r="R35" s="7"/>
-      <c r="S35" s="7"/>
-      <c r="T35" s="7"/>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A36" s="6">
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
+      <c r="O35" s="3"/>
+      <c r="P35" s="3"/>
+      <c r="Q35" s="3"/>
+      <c r="R35" s="3"/>
+      <c r="S35" s="3"/>
+      <c r="T35" s="3"/>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
         <v>35</v>
       </c>
       <c r="B36" t="s">
         <v>51</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D36" t="s">
@@ -2313,7 +2327,7 @@
       <c r="F36" t="s">
         <v>9</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G36" s="5" t="s">
         <v>52</v>
       </c>
       <c r="H36" t="s">
@@ -2322,26 +2336,26 @@
       <c r="I36" t="s">
         <v>82</v>
       </c>
-      <c r="J36" s="7"/>
-      <c r="K36" s="7"/>
-      <c r="L36" s="7"/>
-      <c r="M36" s="7"/>
-      <c r="N36" s="7"/>
-      <c r="O36" s="7"/>
-      <c r="P36" s="7"/>
-      <c r="Q36" s="7"/>
-      <c r="R36" s="7"/>
-      <c r="S36" s="7"/>
-      <c r="T36" s="7"/>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A37" s="6">
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="3"/>
+      <c r="N36" s="3"/>
+      <c r="O36" s="3"/>
+      <c r="P36" s="3"/>
+      <c r="Q36" s="3"/>
+      <c r="R36" s="3"/>
+      <c r="S36" s="3"/>
+      <c r="T36" s="3"/>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
         <v>36</v>
       </c>
       <c r="B37" t="s">
         <v>107</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D37" t="s">
@@ -2353,7 +2367,7 @@
       <c r="F37" t="s">
         <v>9</v>
       </c>
-      <c r="G37" t="s">
+      <c r="G37" s="5" t="s">
         <v>52</v>
       </c>
       <c r="H37" t="s">
@@ -2362,26 +2376,26 @@
       <c r="I37" t="s">
         <v>82</v>
       </c>
-      <c r="J37" s="7"/>
-      <c r="K37" s="7"/>
-      <c r="L37" s="7"/>
-      <c r="M37" s="7"/>
-      <c r="N37" s="7"/>
-      <c r="O37" s="7"/>
-      <c r="P37" s="7"/>
-      <c r="Q37" s="7"/>
-      <c r="R37" s="7"/>
-      <c r="S37" s="7"/>
-      <c r="T37" s="7"/>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A38" s="6">
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="3"/>
+      <c r="O37" s="3"/>
+      <c r="P37" s="3"/>
+      <c r="Q37" s="3"/>
+      <c r="R37" s="3"/>
+      <c r="S37" s="3"/>
+      <c r="T37" s="3"/>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
         <v>37</v>
       </c>
       <c r="B38" t="s">
         <v>108</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="6" t="s">
         <v>136</v>
       </c>
       <c r="D38" t="s">
@@ -2393,7 +2407,7 @@
       <c r="F38" t="s">
         <v>15</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G38" s="5" t="s">
         <v>152</v>
       </c>
       <c r="H38" t="s">
@@ -2402,27 +2416,27 @@
       <c r="I38" t="s">
         <v>82</v>
       </c>
-      <c r="J38" s="7"/>
-      <c r="K38" s="7"/>
-      <c r="L38" s="7"/>
-      <c r="M38" s="7"/>
-      <c r="N38" s="7"/>
-      <c r="O38" s="7"/>
-      <c r="P38" s="7"/>
-      <c r="Q38" s="7"/>
-      <c r="R38" s="7"/>
-      <c r="S38" s="7"/>
-      <c r="T38" s="7"/>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A39" s="6">
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="3"/>
+      <c r="N38" s="3"/>
+      <c r="O38" s="3"/>
+      <c r="P38" s="3"/>
+      <c r="Q38" s="3"/>
+      <c r="R38" s="3"/>
+      <c r="S38" s="3"/>
+      <c r="T38" s="3"/>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
         <v>38</v>
       </c>
       <c r="B39" t="s">
         <v>109</v>
       </c>
-      <c r="C39">
-        <v>3</v>
+      <c r="C39" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="D39" t="s">
         <v>7</v>
@@ -2433,7 +2447,7 @@
       <c r="F39" t="s">
         <v>15</v>
       </c>
-      <c r="G39" t="s">
+      <c r="G39" s="5" t="s">
         <v>152</v>
       </c>
       <c r="H39" t="s">
@@ -2442,27 +2456,27 @@
       <c r="I39" t="s">
         <v>82</v>
       </c>
-      <c r="J39" s="7"/>
-      <c r="K39" s="7"/>
-      <c r="L39" s="7"/>
-      <c r="M39" s="7"/>
-      <c r="N39" s="7"/>
-      <c r="O39" s="7"/>
-      <c r="P39" s="7"/>
-      <c r="Q39" s="7"/>
-      <c r="R39" s="7"/>
-      <c r="S39" s="7"/>
-      <c r="T39" s="7"/>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A40" s="6">
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
+      <c r="O39" s="3"/>
+      <c r="P39" s="3"/>
+      <c r="Q39" s="3"/>
+      <c r="R39" s="3"/>
+      <c r="S39" s="3"/>
+      <c r="T39" s="3"/>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
         <v>39</v>
       </c>
       <c r="B40" t="s">
         <v>110</v>
       </c>
-      <c r="C40">
-        <v>3</v>
+      <c r="C40" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="D40" t="s">
         <v>7</v>
@@ -2473,7 +2487,7 @@
       <c r="F40" t="s">
         <v>15</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G40" s="5" t="s">
         <v>152</v>
       </c>
       <c r="H40" t="s">
@@ -2482,26 +2496,26 @@
       <c r="I40" t="s">
         <v>82</v>
       </c>
-      <c r="J40" s="7"/>
-      <c r="K40" s="7"/>
-      <c r="L40" s="7"/>
-      <c r="M40" s="7"/>
-      <c r="N40" s="7"/>
-      <c r="O40" s="7"/>
-      <c r="P40" s="7"/>
-      <c r="Q40" s="7"/>
-      <c r="R40" s="7"/>
-      <c r="S40" s="7"/>
-      <c r="T40" s="7"/>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A41" s="6">
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="3"/>
+      <c r="N40" s="3"/>
+      <c r="O40" s="3"/>
+      <c r="P40" s="3"/>
+      <c r="Q40" s="3"/>
+      <c r="R40" s="3"/>
+      <c r="S40" s="3"/>
+      <c r="T40" s="3"/>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
         <v>40</v>
       </c>
       <c r="B41" t="s">
         <v>53</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="5" t="s">
         <v>137</v>
       </c>
       <c r="D41" t="s">
@@ -2513,8 +2527,8 @@
       <c r="F41" t="s">
         <v>155</v>
       </c>
-      <c r="G41">
-        <v>40</v>
+      <c r="G41" s="5" t="s">
+        <v>152</v>
       </c>
       <c r="H41" t="s">
         <v>165</v>
@@ -2522,26 +2536,26 @@
       <c r="I41" t="s">
         <v>82</v>
       </c>
-      <c r="J41" s="7"/>
-      <c r="K41" s="7"/>
-      <c r="L41" s="7"/>
-      <c r="M41" s="7"/>
-      <c r="N41" s="7"/>
-      <c r="O41" s="7"/>
-      <c r="P41" s="7"/>
-      <c r="Q41" s="7"/>
-      <c r="R41" s="7"/>
-      <c r="S41" s="7"/>
-      <c r="T41" s="7"/>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A42" s="6">
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
+      <c r="M41" s="3"/>
+      <c r="N41" s="3"/>
+      <c r="O41" s="3"/>
+      <c r="P41" s="3"/>
+      <c r="Q41" s="3"/>
+      <c r="R41" s="3"/>
+      <c r="S41" s="3"/>
+      <c r="T41" s="3"/>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
         <v>41</v>
       </c>
       <c r="B42" t="s">
         <v>111</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C42" s="6" t="s">
         <v>133</v>
       </c>
       <c r="D42" t="s">
@@ -2553,8 +2567,8 @@
       <c r="F42" t="s">
         <v>24</v>
       </c>
-      <c r="G42">
-        <v>42</v>
+      <c r="G42" s="5" t="s">
+        <v>169</v>
       </c>
       <c r="H42" t="s">
         <v>165</v>
@@ -2562,26 +2576,26 @@
       <c r="I42" t="s">
         <v>82</v>
       </c>
-      <c r="J42" s="7"/>
-      <c r="K42" s="7"/>
-      <c r="L42" s="7"/>
-      <c r="M42" s="7"/>
-      <c r="N42" s="7"/>
-      <c r="O42" s="7"/>
-      <c r="P42" s="7"/>
-      <c r="Q42" s="7"/>
-      <c r="R42" s="7"/>
-      <c r="S42" s="7"/>
-      <c r="T42" s="7"/>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A43" s="6">
+      <c r="J42" s="3"/>
+      <c r="K42" s="3"/>
+      <c r="L42" s="3"/>
+      <c r="M42" s="3"/>
+      <c r="N42" s="3"/>
+      <c r="O42" s="3"/>
+      <c r="P42" s="3"/>
+      <c r="Q42" s="3"/>
+      <c r="R42" s="3"/>
+      <c r="S42" s="3"/>
+      <c r="T42" s="3"/>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
         <v>42</v>
       </c>
       <c r="B43" t="s">
         <v>112</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="5" t="s">
         <v>138</v>
       </c>
       <c r="D43" t="s">
@@ -2593,8 +2607,8 @@
       <c r="F43" t="s">
         <v>24</v>
       </c>
-      <c r="G43">
-        <v>42</v>
+      <c r="G43" s="5" t="s">
+        <v>169</v>
       </c>
       <c r="H43" t="s">
         <v>165</v>
@@ -2602,26 +2616,26 @@
       <c r="I43" t="s">
         <v>82</v>
       </c>
-      <c r="J43" s="7"/>
-      <c r="K43" s="7"/>
-      <c r="L43" s="7"/>
-      <c r="M43" s="7"/>
-      <c r="N43" s="7"/>
-      <c r="O43" s="7"/>
-      <c r="P43" s="7"/>
-      <c r="Q43" s="7"/>
-      <c r="R43" s="7"/>
-      <c r="S43" s="7"/>
-      <c r="T43" s="7"/>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A44" s="6">
+      <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
+      <c r="L43" s="3"/>
+      <c r="M43" s="3"/>
+      <c r="N43" s="3"/>
+      <c r="O43" s="3"/>
+      <c r="P43" s="3"/>
+      <c r="Q43" s="3"/>
+      <c r="R43" s="3"/>
+      <c r="S43" s="3"/>
+      <c r="T43" s="3"/>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
         <v>43</v>
       </c>
       <c r="B44" t="s">
         <v>113</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D44" t="s">
@@ -2633,8 +2647,8 @@
       <c r="F44" t="s">
         <v>155</v>
       </c>
-      <c r="G44">
-        <v>43</v>
+      <c r="G44" s="5" t="s">
+        <v>170</v>
       </c>
       <c r="H44" t="s">
         <v>165</v>
@@ -2642,26 +2656,26 @@
       <c r="I44" t="s">
         <v>82</v>
       </c>
-      <c r="J44" s="7"/>
-      <c r="K44" s="7"/>
-      <c r="L44" s="7"/>
-      <c r="M44" s="7"/>
-      <c r="N44" s="7"/>
-      <c r="O44" s="7"/>
-      <c r="P44" s="7"/>
-      <c r="Q44" s="7"/>
-      <c r="R44" s="7"/>
-      <c r="S44" s="7"/>
-      <c r="T44" s="7"/>
-    </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A45" s="6">
+      <c r="J44" s="3"/>
+      <c r="K44" s="3"/>
+      <c r="L44" s="3"/>
+      <c r="M44" s="3"/>
+      <c r="N44" s="3"/>
+      <c r="O44" s="3"/>
+      <c r="P44" s="3"/>
+      <c r="Q44" s="3"/>
+      <c r="R44" s="3"/>
+      <c r="S44" s="3"/>
+      <c r="T44" s="3"/>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
         <v>44</v>
       </c>
       <c r="B45" t="s">
         <v>55</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C45" s="6" t="s">
         <v>139</v>
       </c>
       <c r="D45" t="s">
@@ -2673,8 +2687,8 @@
       <c r="F45" t="s">
         <v>28</v>
       </c>
-      <c r="G45">
-        <v>43</v>
+      <c r="G45" s="5" t="s">
+        <v>170</v>
       </c>
       <c r="H45" t="s">
         <v>165</v>
@@ -2682,27 +2696,27 @@
       <c r="I45" t="s">
         <v>82</v>
       </c>
-      <c r="J45" s="7"/>
-      <c r="K45" s="7"/>
-      <c r="L45" s="7"/>
-      <c r="M45" s="7"/>
-      <c r="N45" s="7"/>
-      <c r="O45" s="7"/>
-      <c r="P45" s="7"/>
-      <c r="Q45" s="7"/>
-      <c r="R45" s="7"/>
-      <c r="S45" s="7"/>
-      <c r="T45" s="7"/>
-    </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A46" s="6">
+      <c r="J45" s="3"/>
+      <c r="K45" s="3"/>
+      <c r="L45" s="3"/>
+      <c r="M45" s="3"/>
+      <c r="N45" s="3"/>
+      <c r="O45" s="3"/>
+      <c r="P45" s="3"/>
+      <c r="Q45" s="3"/>
+      <c r="R45" s="3"/>
+      <c r="S45" s="3"/>
+      <c r="T45" s="3"/>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
         <v>45</v>
       </c>
       <c r="B46" t="s">
         <v>114</v>
       </c>
-      <c r="C46">
-        <v>2</v>
+      <c r="C46" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D46" t="s">
         <v>32</v>
@@ -2713,8 +2727,8 @@
       <c r="F46" t="s">
         <v>28</v>
       </c>
-      <c r="G46">
-        <v>44</v>
+      <c r="G46" s="5" t="s">
+        <v>171</v>
       </c>
       <c r="H46" t="s">
         <v>166</v>
@@ -2722,26 +2736,26 @@
       <c r="I46" t="s">
         <v>82</v>
       </c>
-      <c r="J46" s="7"/>
-      <c r="K46" s="7"/>
-      <c r="L46" s="7"/>
-      <c r="M46" s="7"/>
-      <c r="N46" s="7"/>
-      <c r="O46" s="7"/>
-      <c r="P46" s="7"/>
-      <c r="Q46" s="7"/>
-      <c r="R46" s="7"/>
-      <c r="S46" s="7"/>
-      <c r="T46" s="7"/>
-    </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A47" s="6">
+      <c r="J46" s="3"/>
+      <c r="K46" s="3"/>
+      <c r="L46" s="3"/>
+      <c r="M46" s="3"/>
+      <c r="N46" s="3"/>
+      <c r="O46" s="3"/>
+      <c r="P46" s="3"/>
+      <c r="Q46" s="3"/>
+      <c r="R46" s="3"/>
+      <c r="S46" s="3"/>
+      <c r="T46" s="3"/>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
         <v>46</v>
       </c>
       <c r="B47" t="s">
         <v>115</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D47" t="s">
@@ -2753,8 +2767,8 @@
       <c r="F47" t="s">
         <v>155</v>
       </c>
-      <c r="G47">
-        <v>45</v>
+      <c r="G47" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="H47" t="s">
         <v>165</v>
@@ -2762,26 +2776,26 @@
       <c r="I47" t="s">
         <v>82</v>
       </c>
-      <c r="J47" s="7"/>
-      <c r="K47" s="7"/>
-      <c r="L47" s="7"/>
-      <c r="M47" s="7"/>
-      <c r="N47" s="7"/>
-      <c r="O47" s="7"/>
-      <c r="P47" s="7"/>
-      <c r="Q47" s="7"/>
-      <c r="R47" s="7"/>
-      <c r="S47" s="7"/>
-      <c r="T47" s="7"/>
-    </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A48" s="6">
+      <c r="J47" s="3"/>
+      <c r="K47" s="3"/>
+      <c r="L47" s="3"/>
+      <c r="M47" s="3"/>
+      <c r="N47" s="3"/>
+      <c r="O47" s="3"/>
+      <c r="P47" s="3"/>
+      <c r="Q47" s="3"/>
+      <c r="R47" s="3"/>
+      <c r="S47" s="3"/>
+      <c r="T47" s="3"/>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
         <v>47</v>
       </c>
       <c r="B48" t="s">
         <v>116</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D48" t="s">
@@ -2793,7 +2807,7 @@
       <c r="F48" t="s">
         <v>15</v>
       </c>
-      <c r="G48" t="s">
+      <c r="G48" s="5" t="s">
         <v>56</v>
       </c>
       <c r="H48" t="s">
@@ -2802,26 +2816,26 @@
       <c r="I48" t="s">
         <v>82</v>
       </c>
-      <c r="J48" s="7"/>
-      <c r="K48" s="7"/>
-      <c r="L48" s="7"/>
-      <c r="M48" s="7"/>
-      <c r="N48" s="7"/>
-      <c r="O48" s="7"/>
-      <c r="P48" s="7"/>
-      <c r="Q48" s="7"/>
-      <c r="R48" s="7"/>
-      <c r="S48" s="7"/>
-      <c r="T48" s="7"/>
-    </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A49" s="6">
+      <c r="J48" s="3"/>
+      <c r="K48" s="3"/>
+      <c r="L48" s="3"/>
+      <c r="M48" s="3"/>
+      <c r="N48" s="3"/>
+      <c r="O48" s="3"/>
+      <c r="P48" s="3"/>
+      <c r="Q48" s="3"/>
+      <c r="R48" s="3"/>
+      <c r="S48" s="3"/>
+      <c r="T48" s="3"/>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
         <v>48</v>
       </c>
       <c r="B49" t="s">
         <v>117</v>
       </c>
-      <c r="C49" s="5" t="s">
+      <c r="C49" s="6" t="s">
         <v>148</v>
       </c>
       <c r="D49" t="s">
@@ -2833,7 +2847,7 @@
       <c r="F49" t="s">
         <v>57</v>
       </c>
-      <c r="G49" t="s">
+      <c r="G49" s="5" t="s">
         <v>56</v>
       </c>
       <c r="H49" t="s">
@@ -2842,26 +2856,26 @@
       <c r="I49" t="s">
         <v>82</v>
       </c>
-      <c r="J49" s="7"/>
-      <c r="K49" s="7"/>
-      <c r="L49" s="7"/>
-      <c r="M49" s="7"/>
-      <c r="N49" s="7"/>
-      <c r="O49" s="7"/>
-      <c r="P49" s="7"/>
-      <c r="Q49" s="7"/>
-      <c r="R49" s="7"/>
-      <c r="S49" s="7"/>
-      <c r="T49" s="7"/>
-    </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A50" s="6">
+      <c r="J49" s="3"/>
+      <c r="K49" s="3"/>
+      <c r="L49" s="3"/>
+      <c r="M49" s="3"/>
+      <c r="N49" s="3"/>
+      <c r="O49" s="3"/>
+      <c r="P49" s="3"/>
+      <c r="Q49" s="3"/>
+      <c r="R49" s="3"/>
+      <c r="S49" s="3"/>
+      <c r="T49" s="3"/>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
         <v>49</v>
       </c>
       <c r="B50" t="s">
         <v>118</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D50" t="s">
@@ -2873,7 +2887,7 @@
       <c r="F50" t="s">
         <v>57</v>
       </c>
-      <c r="G50" t="s">
+      <c r="G50" s="5" t="s">
         <v>58</v>
       </c>
       <c r="H50" t="s">
@@ -2882,26 +2896,26 @@
       <c r="I50" t="s">
         <v>82</v>
       </c>
-      <c r="J50" s="7"/>
-      <c r="K50" s="7"/>
-      <c r="L50" s="7"/>
-      <c r="M50" s="7"/>
-      <c r="N50" s="7"/>
-      <c r="O50" s="7"/>
-      <c r="P50" s="7"/>
-      <c r="Q50" s="7"/>
-      <c r="R50" s="7"/>
-      <c r="S50" s="7"/>
-      <c r="T50" s="7"/>
-    </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A51" s="6">
+      <c r="J50" s="3"/>
+      <c r="K50" s="3"/>
+      <c r="L50" s="3"/>
+      <c r="M50" s="3"/>
+      <c r="N50" s="3"/>
+      <c r="O50" s="3"/>
+      <c r="P50" s="3"/>
+      <c r="Q50" s="3"/>
+      <c r="R50" s="3"/>
+      <c r="S50" s="3"/>
+      <c r="T50" s="3"/>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
         <v>50</v>
       </c>
       <c r="B51" t="s">
         <v>59</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D51" t="s">
@@ -2913,7 +2927,7 @@
       <c r="F51" t="s">
         <v>24</v>
       </c>
-      <c r="G51" t="s">
+      <c r="G51" s="5" t="s">
         <v>58</v>
       </c>
       <c r="H51" t="s">
@@ -2922,27 +2936,27 @@
       <c r="I51" t="s">
         <v>82</v>
       </c>
-      <c r="J51" s="7"/>
-      <c r="K51" s="7"/>
-      <c r="L51" s="7"/>
-      <c r="M51" s="7"/>
-      <c r="N51" s="7"/>
-      <c r="O51" s="7"/>
-      <c r="P51" s="7"/>
-      <c r="Q51" s="7"/>
-      <c r="R51" s="7"/>
-      <c r="S51" s="7"/>
-      <c r="T51" s="7"/>
-    </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A52" s="6">
+      <c r="J51" s="3"/>
+      <c r="K51" s="3"/>
+      <c r="L51" s="3"/>
+      <c r="M51" s="3"/>
+      <c r="N51" s="3"/>
+      <c r="O51" s="3"/>
+      <c r="P51" s="3"/>
+      <c r="Q51" s="3"/>
+      <c r="R51" s="3"/>
+      <c r="S51" s="3"/>
+      <c r="T51" s="3"/>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
         <v>51</v>
       </c>
       <c r="B52" t="s">
         <v>119</v>
       </c>
-      <c r="C52">
-        <v>3</v>
+      <c r="C52" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="D52" t="s">
         <v>7</v>
@@ -2953,7 +2967,7 @@
       <c r="F52" t="s">
         <v>15</v>
       </c>
-      <c r="G52" t="s">
+      <c r="G52" s="5" t="s">
         <v>156</v>
       </c>
       <c r="H52" t="s">
@@ -2962,27 +2976,27 @@
       <c r="I52" t="s">
         <v>82</v>
       </c>
-      <c r="J52" s="7"/>
-      <c r="K52" s="7"/>
-      <c r="L52" s="7"/>
-      <c r="M52" s="7"/>
-      <c r="N52" s="7"/>
-      <c r="O52" s="7"/>
-      <c r="P52" s="7"/>
-      <c r="Q52" s="7"/>
-      <c r="R52" s="7"/>
-      <c r="S52" s="7"/>
-      <c r="T52" s="7"/>
-    </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A53" s="6">
+      <c r="J52" s="3"/>
+      <c r="K52" s="3"/>
+      <c r="L52" s="3"/>
+      <c r="M52" s="3"/>
+      <c r="N52" s="3"/>
+      <c r="O52" s="3"/>
+      <c r="P52" s="3"/>
+      <c r="Q52" s="3"/>
+      <c r="R52" s="3"/>
+      <c r="S52" s="3"/>
+      <c r="T52" s="3"/>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
         <v>52</v>
       </c>
       <c r="B53" t="s">
         <v>120</v>
       </c>
-      <c r="C53">
-        <v>3</v>
+      <c r="C53" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="D53" t="s">
         <v>7</v>
@@ -2993,7 +3007,7 @@
       <c r="F53" t="s">
         <v>15</v>
       </c>
-      <c r="G53" t="s">
+      <c r="G53" s="5" t="s">
         <v>156</v>
       </c>
       <c r="H53" t="s">
@@ -3002,26 +3016,26 @@
       <c r="I53" t="s">
         <v>82</v>
       </c>
-      <c r="J53" s="7"/>
-      <c r="K53" s="7"/>
-      <c r="L53" s="7"/>
-      <c r="M53" s="7"/>
-      <c r="N53" s="7"/>
-      <c r="O53" s="7"/>
-      <c r="P53" s="7"/>
-      <c r="Q53" s="7"/>
-      <c r="R53" s="7"/>
-      <c r="S53" s="7"/>
-      <c r="T53" s="7"/>
-    </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A54" s="6">
+      <c r="J53" s="3"/>
+      <c r="K53" s="3"/>
+      <c r="L53" s="3"/>
+      <c r="M53" s="3"/>
+      <c r="N53" s="3"/>
+      <c r="O53" s="3"/>
+      <c r="P53" s="3"/>
+      <c r="Q53" s="3"/>
+      <c r="R53" s="3"/>
+      <c r="S53" s="3"/>
+      <c r="T53" s="3"/>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
         <v>53</v>
       </c>
       <c r="B54" t="s">
         <v>60</v>
       </c>
-      <c r="C54" s="5" t="s">
+      <c r="C54" s="6" t="s">
         <v>140</v>
       </c>
       <c r="D54" t="s">
@@ -3033,7 +3047,7 @@
       <c r="F54" t="s">
         <v>9</v>
       </c>
-      <c r="G54" t="s">
+      <c r="G54" s="5" t="s">
         <v>156</v>
       </c>
       <c r="H54" t="s">
@@ -3042,26 +3056,26 @@
       <c r="I54" t="s">
         <v>82</v>
       </c>
-      <c r="J54" s="7"/>
-      <c r="K54" s="7"/>
-      <c r="L54" s="7"/>
-      <c r="M54" s="7"/>
-      <c r="N54" s="7"/>
-      <c r="O54" s="7"/>
-      <c r="P54" s="7"/>
-      <c r="Q54" s="7"/>
-      <c r="R54" s="7"/>
-      <c r="S54" s="7"/>
-      <c r="T54" s="7"/>
-    </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A55" s="6">
+      <c r="J54" s="3"/>
+      <c r="K54" s="3"/>
+      <c r="L54" s="3"/>
+      <c r="M54" s="3"/>
+      <c r="N54" s="3"/>
+      <c r="O54" s="3"/>
+      <c r="P54" s="3"/>
+      <c r="Q54" s="3"/>
+      <c r="R54" s="3"/>
+      <c r="S54" s="3"/>
+      <c r="T54" s="3"/>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
         <v>54</v>
       </c>
       <c r="B55" t="s">
         <v>61</v>
       </c>
-      <c r="C55" s="5" t="s">
+      <c r="C55" s="6" t="s">
         <v>140</v>
       </c>
       <c r="D55" t="s">
@@ -3073,7 +3087,7 @@
       <c r="F55" t="s">
         <v>28</v>
       </c>
-      <c r="G55" t="s">
+      <c r="G55" s="5" t="s">
         <v>157</v>
       </c>
       <c r="H55" t="s">
@@ -3082,26 +3096,26 @@
       <c r="I55" t="s">
         <v>82</v>
       </c>
-      <c r="J55" s="7"/>
-      <c r="K55" s="7"/>
-      <c r="L55" s="7"/>
-      <c r="M55" s="7"/>
-      <c r="N55" s="7"/>
-      <c r="O55" s="7"/>
-      <c r="P55" s="7"/>
-      <c r="Q55" s="7"/>
-      <c r="R55" s="7"/>
-      <c r="S55" s="7"/>
-      <c r="T55" s="7"/>
-    </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A56" s="6">
+      <c r="J55" s="3"/>
+      <c r="K55" s="3"/>
+      <c r="L55" s="3"/>
+      <c r="M55" s="3"/>
+      <c r="N55" s="3"/>
+      <c r="O55" s="3"/>
+      <c r="P55" s="3"/>
+      <c r="Q55" s="3"/>
+      <c r="R55" s="3"/>
+      <c r="S55" s="3"/>
+      <c r="T55" s="3"/>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A56" s="2">
         <v>55</v>
       </c>
       <c r="B56" t="s">
         <v>62</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D56" t="s">
@@ -3113,8 +3127,8 @@
       <c r="F56" t="s">
         <v>153</v>
       </c>
-      <c r="G56">
-        <v>50</v>
+      <c r="G56" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="H56" t="s">
         <v>165</v>
@@ -3122,26 +3136,26 @@
       <c r="I56" t="s">
         <v>82</v>
       </c>
-      <c r="J56" s="7"/>
-      <c r="K56" s="7"/>
-      <c r="L56" s="7"/>
-      <c r="M56" s="7"/>
-      <c r="N56" s="7"/>
-      <c r="O56" s="7"/>
-      <c r="P56" s="7"/>
-      <c r="Q56" s="7"/>
-      <c r="R56" s="7"/>
-      <c r="S56" s="7"/>
-      <c r="T56" s="7"/>
-    </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A57" s="6">
+      <c r="J56" s="3"/>
+      <c r="K56" s="3"/>
+      <c r="L56" s="3"/>
+      <c r="M56" s="3"/>
+      <c r="N56" s="3"/>
+      <c r="O56" s="3"/>
+      <c r="P56" s="3"/>
+      <c r="Q56" s="3"/>
+      <c r="R56" s="3"/>
+      <c r="S56" s="3"/>
+      <c r="T56" s="3"/>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
         <v>56</v>
       </c>
       <c r="B57" t="s">
         <v>121</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D57" t="s">
@@ -3153,7 +3167,7 @@
       <c r="F57" t="s">
         <v>24</v>
       </c>
-      <c r="G57" t="s">
+      <c r="G57" s="5" t="s">
         <v>63</v>
       </c>
       <c r="H57" t="s">
@@ -3162,26 +3176,26 @@
       <c r="I57" t="s">
         <v>82</v>
       </c>
-      <c r="J57" s="7"/>
-      <c r="K57" s="7"/>
-      <c r="L57" s="7"/>
-      <c r="M57" s="7"/>
-      <c r="N57" s="7"/>
-      <c r="O57" s="7"/>
-      <c r="P57" s="7"/>
-      <c r="Q57" s="7"/>
-      <c r="R57" s="7"/>
-      <c r="S57" s="7"/>
-      <c r="T57" s="7"/>
-    </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A58" s="6">
+      <c r="J57" s="3"/>
+      <c r="K57" s="3"/>
+      <c r="L57" s="3"/>
+      <c r="M57" s="3"/>
+      <c r="N57" s="3"/>
+      <c r="O57" s="3"/>
+      <c r="P57" s="3"/>
+      <c r="Q57" s="3"/>
+      <c r="R57" s="3"/>
+      <c r="S57" s="3"/>
+      <c r="T57" s="3"/>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
         <v>57</v>
       </c>
       <c r="B58" t="s">
         <v>54</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D58" t="s">
@@ -3193,7 +3207,7 @@
       <c r="F58" t="s">
         <v>15</v>
       </c>
-      <c r="G58" t="s">
+      <c r="G58" s="5" t="s">
         <v>63</v>
       </c>
       <c r="H58" t="s">
@@ -3202,26 +3216,26 @@
       <c r="I58" t="s">
         <v>82</v>
       </c>
-      <c r="J58" s="7"/>
-      <c r="K58" s="7"/>
-      <c r="L58" s="7"/>
-      <c r="M58" s="7"/>
-      <c r="N58" s="7"/>
-      <c r="O58" s="7"/>
-      <c r="P58" s="7"/>
-      <c r="Q58" s="7"/>
-      <c r="R58" s="7"/>
-      <c r="S58" s="7"/>
-      <c r="T58" s="7"/>
-    </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A59" s="6">
+      <c r="J58" s="3"/>
+      <c r="K58" s="3"/>
+      <c r="L58" s="3"/>
+      <c r="M58" s="3"/>
+      <c r="N58" s="3"/>
+      <c r="O58" s="3"/>
+      <c r="P58" s="3"/>
+      <c r="Q58" s="3"/>
+      <c r="R58" s="3"/>
+      <c r="S58" s="3"/>
+      <c r="T58" s="3"/>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
         <v>58</v>
       </c>
       <c r="B59" t="s">
         <v>122</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D59" t="s">
@@ -3233,7 +3247,7 @@
       <c r="F59" t="s">
         <v>28</v>
       </c>
-      <c r="G59" t="s">
+      <c r="G59" s="5" t="s">
         <v>63</v>
       </c>
       <c r="H59" t="s">
@@ -3242,26 +3256,26 @@
       <c r="I59" t="s">
         <v>82</v>
       </c>
-      <c r="J59" s="7"/>
-      <c r="K59" s="7"/>
-      <c r="L59" s="7"/>
-      <c r="M59" s="7"/>
-      <c r="N59" s="7"/>
-      <c r="O59" s="7"/>
-      <c r="P59" s="7"/>
-      <c r="Q59" s="7"/>
-      <c r="R59" s="7"/>
-      <c r="S59" s="7"/>
-      <c r="T59" s="7"/>
-    </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A60" s="6">
+      <c r="J59" s="3"/>
+      <c r="K59" s="3"/>
+      <c r="L59" s="3"/>
+      <c r="M59" s="3"/>
+      <c r="N59" s="3"/>
+      <c r="O59" s="3"/>
+      <c r="P59" s="3"/>
+      <c r="Q59" s="3"/>
+      <c r="R59" s="3"/>
+      <c r="S59" s="3"/>
+      <c r="T59" s="3"/>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A60" s="2">
         <v>59</v>
       </c>
       <c r="B60" t="s">
         <v>123</v>
       </c>
-      <c r="C60" s="5" t="s">
+      <c r="C60" s="6" t="s">
         <v>141</v>
       </c>
       <c r="D60" t="s">
@@ -3273,7 +3287,7 @@
       <c r="F60" t="s">
         <v>9</v>
       </c>
-      <c r="G60" t="s">
+      <c r="G60" s="5" t="s">
         <v>158</v>
       </c>
       <c r="H60" t="s">
@@ -3282,26 +3296,26 @@
       <c r="I60" t="s">
         <v>82</v>
       </c>
-      <c r="J60" s="7"/>
-      <c r="K60" s="7"/>
-      <c r="L60" s="7"/>
-      <c r="M60" s="7"/>
-      <c r="N60" s="7"/>
-      <c r="O60" s="7"/>
-      <c r="P60" s="7"/>
-      <c r="Q60" s="7"/>
-      <c r="R60" s="7"/>
-      <c r="S60" s="7"/>
-      <c r="T60" s="7"/>
-    </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A61" s="6">
+      <c r="J60" s="3"/>
+      <c r="K60" s="3"/>
+      <c r="L60" s="3"/>
+      <c r="M60" s="3"/>
+      <c r="N60" s="3"/>
+      <c r="O60" s="3"/>
+      <c r="P60" s="3"/>
+      <c r="Q60" s="3"/>
+      <c r="R60" s="3"/>
+      <c r="S60" s="3"/>
+      <c r="T60" s="3"/>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A61" s="2">
         <v>60</v>
       </c>
       <c r="B61" t="s">
         <v>64</v>
       </c>
-      <c r="C61" s="5" t="s">
+      <c r="C61" s="6" t="s">
         <v>142</v>
       </c>
       <c r="D61" t="s">
@@ -3313,8 +3327,8 @@
       <c r="F61" t="s">
         <v>161</v>
       </c>
-      <c r="G61">
-        <v>52</v>
+      <c r="G61" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="H61" t="s">
         <v>166</v>
@@ -3322,26 +3336,26 @@
       <c r="I61" t="s">
         <v>82</v>
       </c>
-      <c r="J61" s="7"/>
-      <c r="K61" s="7"/>
-      <c r="L61" s="7"/>
-      <c r="M61" s="7"/>
-      <c r="N61" s="7"/>
-      <c r="O61" s="7"/>
-      <c r="P61" s="7"/>
-      <c r="Q61" s="7"/>
-      <c r="R61" s="7"/>
-      <c r="S61" s="7"/>
-      <c r="T61" s="7"/>
-    </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A62" s="6">
+      <c r="J61" s="3"/>
+      <c r="K61" s="3"/>
+      <c r="L61" s="3"/>
+      <c r="M61" s="3"/>
+      <c r="N61" s="3"/>
+      <c r="O61" s="3"/>
+      <c r="P61" s="3"/>
+      <c r="Q61" s="3"/>
+      <c r="R61" s="3"/>
+      <c r="S61" s="3"/>
+      <c r="T61" s="3"/>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
         <v>61</v>
       </c>
       <c r="B62" t="s">
         <v>65</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D62" t="s">
@@ -3353,7 +3367,7 @@
       <c r="F62" t="s">
         <v>9</v>
       </c>
-      <c r="G62" t="s">
+      <c r="G62" s="5" t="s">
         <v>66</v>
       </c>
       <c r="H62" t="s">
@@ -3362,26 +3376,26 @@
       <c r="I62" t="s">
         <v>82</v>
       </c>
-      <c r="J62" s="7"/>
-      <c r="K62" s="7"/>
-      <c r="L62" s="7"/>
-      <c r="M62" s="7"/>
-      <c r="N62" s="7"/>
-      <c r="O62" s="7"/>
-      <c r="P62" s="7"/>
-      <c r="Q62" s="7"/>
-      <c r="R62" s="7"/>
-      <c r="S62" s="7"/>
-      <c r="T62" s="7"/>
-    </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A63" s="6">
+      <c r="J62" s="3"/>
+      <c r="K62" s="3"/>
+      <c r="L62" s="3"/>
+      <c r="M62" s="3"/>
+      <c r="N62" s="3"/>
+      <c r="O62" s="3"/>
+      <c r="P62" s="3"/>
+      <c r="Q62" s="3"/>
+      <c r="R62" s="3"/>
+      <c r="S62" s="3"/>
+      <c r="T62" s="3"/>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
         <v>62</v>
       </c>
       <c r="B63" t="s">
         <v>124</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D63" t="s">
@@ -3393,7 +3407,7 @@
       <c r="F63" t="s">
         <v>57</v>
       </c>
-      <c r="G63" t="s">
+      <c r="G63" s="5" t="s">
         <v>66</v>
       </c>
       <c r="H63" t="s">
@@ -3402,26 +3416,26 @@
       <c r="I63" t="s">
         <v>82</v>
       </c>
-      <c r="J63" s="7"/>
-      <c r="K63" s="7"/>
-      <c r="L63" s="7"/>
-      <c r="M63" s="7"/>
-      <c r="N63" s="7"/>
-      <c r="O63" s="7"/>
-      <c r="P63" s="7"/>
-      <c r="Q63" s="7"/>
-      <c r="R63" s="7"/>
-      <c r="S63" s="7"/>
-      <c r="T63" s="7"/>
-    </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A64" s="6">
+      <c r="J63" s="3"/>
+      <c r="K63" s="3"/>
+      <c r="L63" s="3"/>
+      <c r="M63" s="3"/>
+      <c r="N63" s="3"/>
+      <c r="O63" s="3"/>
+      <c r="P63" s="3"/>
+      <c r="Q63" s="3"/>
+      <c r="R63" s="3"/>
+      <c r="S63" s="3"/>
+      <c r="T63" s="3"/>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
         <v>63</v>
       </c>
       <c r="B64" t="s">
         <v>125</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D64" t="s">
@@ -3433,7 +3447,7 @@
       <c r="F64" t="s">
         <v>9</v>
       </c>
-      <c r="G64" t="s">
+      <c r="G64" s="5" t="s">
         <v>67</v>
       </c>
       <c r="H64" t="s">
@@ -3442,26 +3456,26 @@
       <c r="I64" t="s">
         <v>82</v>
       </c>
-      <c r="J64" s="7"/>
-      <c r="K64" s="7"/>
-      <c r="L64" s="7"/>
-      <c r="M64" s="7"/>
-      <c r="N64" s="7"/>
-      <c r="O64" s="7"/>
-      <c r="P64" s="7"/>
-      <c r="Q64" s="7"/>
-      <c r="R64" s="7"/>
-      <c r="S64" s="7"/>
-      <c r="T64" s="7"/>
-    </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A65" s="6">
+      <c r="J64" s="3"/>
+      <c r="K64" s="3"/>
+      <c r="L64" s="3"/>
+      <c r="M64" s="3"/>
+      <c r="N64" s="3"/>
+      <c r="O64" s="3"/>
+      <c r="P64" s="3"/>
+      <c r="Q64" s="3"/>
+      <c r="R64" s="3"/>
+      <c r="S64" s="3"/>
+      <c r="T64" s="3"/>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A65" s="2">
         <v>64</v>
       </c>
       <c r="B65" t="s">
         <v>68</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D65" t="s">
@@ -3473,7 +3487,7 @@
       <c r="F65" t="s">
         <v>24</v>
       </c>
-      <c r="G65" t="s">
+      <c r="G65" s="5" t="s">
         <v>69</v>
       </c>
       <c r="H65" t="s">
@@ -3482,26 +3496,26 @@
       <c r="I65" t="s">
         <v>82</v>
       </c>
-      <c r="J65" s="7"/>
-      <c r="K65" s="7"/>
-      <c r="L65" s="7"/>
-      <c r="M65" s="7"/>
-      <c r="N65" s="7"/>
-      <c r="O65" s="7"/>
-      <c r="P65" s="7"/>
-      <c r="Q65" s="7"/>
-      <c r="R65" s="7"/>
-      <c r="S65" s="7"/>
-      <c r="T65" s="7"/>
-    </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A66" s="6">
+      <c r="J65" s="3"/>
+      <c r="K65" s="3"/>
+      <c r="L65" s="3"/>
+      <c r="M65" s="3"/>
+      <c r="N65" s="3"/>
+      <c r="O65" s="3"/>
+      <c r="P65" s="3"/>
+      <c r="Q65" s="3"/>
+      <c r="R65" s="3"/>
+      <c r="S65" s="3"/>
+      <c r="T65" s="3"/>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A66" s="2">
         <v>65</v>
       </c>
       <c r="B66" t="s">
         <v>70</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D66" t="s">
@@ -3513,7 +3527,7 @@
       <c r="F66" t="s">
         <v>9</v>
       </c>
-      <c r="G66" t="s">
+      <c r="G66" s="5" t="s">
         <v>69</v>
       </c>
       <c r="H66" t="s">
@@ -3522,26 +3536,26 @@
       <c r="I66" t="s">
         <v>82</v>
       </c>
-      <c r="J66" s="7"/>
-      <c r="K66" s="7"/>
-      <c r="L66" s="7"/>
-      <c r="M66" s="7"/>
-      <c r="N66" s="7"/>
-      <c r="O66" s="7"/>
-      <c r="P66" s="7"/>
-      <c r="Q66" s="7"/>
-      <c r="R66" s="7"/>
-      <c r="S66" s="7"/>
-      <c r="T66" s="7"/>
-    </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A67" s="6">
+      <c r="J66" s="3"/>
+      <c r="K66" s="3"/>
+      <c r="L66" s="3"/>
+      <c r="M66" s="3"/>
+      <c r="N66" s="3"/>
+      <c r="O66" s="3"/>
+      <c r="P66" s="3"/>
+      <c r="Q66" s="3"/>
+      <c r="R66" s="3"/>
+      <c r="S66" s="3"/>
+      <c r="T66" s="3"/>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A67" s="2">
         <v>66</v>
       </c>
       <c r="B67" t="s">
         <v>71</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" s="5" t="s">
         <v>27</v>
       </c>
       <c r="D67" t="s">
@@ -3553,7 +3567,7 @@
       <c r="F67" t="s">
         <v>9</v>
       </c>
-      <c r="G67" t="s">
+      <c r="G67" s="5" t="s">
         <v>69</v>
       </c>
       <c r="H67" t="s">
@@ -3562,26 +3576,26 @@
       <c r="I67" t="s">
         <v>82</v>
       </c>
-      <c r="J67" s="7"/>
-      <c r="K67" s="7"/>
-      <c r="L67" s="7"/>
-      <c r="M67" s="7"/>
-      <c r="N67" s="7"/>
-      <c r="O67" s="7"/>
-      <c r="P67" s="7"/>
-      <c r="Q67" s="7"/>
-      <c r="R67" s="7"/>
-      <c r="S67" s="7"/>
-      <c r="T67" s="7"/>
-    </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A68" s="6">
+      <c r="J67" s="3"/>
+      <c r="K67" s="3"/>
+      <c r="L67" s="3"/>
+      <c r="M67" s="3"/>
+      <c r="N67" s="3"/>
+      <c r="O67" s="3"/>
+      <c r="P67" s="3"/>
+      <c r="Q67" s="3"/>
+      <c r="R67" s="3"/>
+      <c r="S67" s="3"/>
+      <c r="T67" s="3"/>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A68" s="2">
         <v>67</v>
       </c>
       <c r="B68" t="s">
         <v>72</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D68" t="s">
@@ -3593,7 +3607,7 @@
       <c r="F68" t="s">
         <v>9</v>
       </c>
-      <c r="G68" t="s">
+      <c r="G68" s="5" t="s">
         <v>69</v>
       </c>
       <c r="H68" t="s">
@@ -3602,26 +3616,26 @@
       <c r="I68" t="s">
         <v>82</v>
       </c>
-      <c r="J68" s="7"/>
-      <c r="K68" s="7"/>
-      <c r="L68" s="7"/>
-      <c r="M68" s="7"/>
-      <c r="N68" s="7"/>
-      <c r="O68" s="7"/>
-      <c r="P68" s="7"/>
-      <c r="Q68" s="7"/>
-      <c r="R68" s="7"/>
-      <c r="S68" s="7"/>
-      <c r="T68" s="7"/>
-    </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A69" s="6">
+      <c r="J68" s="3"/>
+      <c r="K68" s="3"/>
+      <c r="L68" s="3"/>
+      <c r="M68" s="3"/>
+      <c r="N68" s="3"/>
+      <c r="O68" s="3"/>
+      <c r="P68" s="3"/>
+      <c r="Q68" s="3"/>
+      <c r="R68" s="3"/>
+      <c r="S68" s="3"/>
+      <c r="T68" s="3"/>
+    </row>
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A69" s="2">
         <v>68</v>
       </c>
       <c r="B69" t="s">
         <v>73</v>
       </c>
-      <c r="C69" s="5" t="s">
+      <c r="C69" s="6" t="s">
         <v>143</v>
       </c>
       <c r="D69" t="s">
@@ -3633,7 +3647,7 @@
       <c r="F69" t="s">
         <v>24</v>
       </c>
-      <c r="G69" t="s">
+      <c r="G69" s="5" t="s">
         <v>159</v>
       </c>
       <c r="H69" t="s">
@@ -3642,26 +3656,26 @@
       <c r="I69" t="s">
         <v>82</v>
       </c>
-      <c r="J69" s="7"/>
-      <c r="K69" s="7"/>
-      <c r="L69" s="7"/>
-      <c r="M69" s="7"/>
-      <c r="N69" s="7"/>
-      <c r="O69" s="7"/>
-      <c r="P69" s="7"/>
-      <c r="Q69" s="7"/>
-      <c r="R69" s="7"/>
-      <c r="S69" s="7"/>
-      <c r="T69" s="7"/>
-    </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A70" s="6">
+      <c r="J69" s="3"/>
+      <c r="K69" s="3"/>
+      <c r="L69" s="3"/>
+      <c r="M69" s="3"/>
+      <c r="N69" s="3"/>
+      <c r="O69" s="3"/>
+      <c r="P69" s="3"/>
+      <c r="Q69" s="3"/>
+      <c r="R69" s="3"/>
+      <c r="S69" s="3"/>
+      <c r="T69" s="3"/>
+    </row>
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A70" s="2">
         <v>69</v>
       </c>
       <c r="B70" t="s">
         <v>74</v>
       </c>
-      <c r="C70" s="5" t="s">
+      <c r="C70" s="6" t="s">
         <v>144</v>
       </c>
       <c r="D70" t="s">
@@ -3673,7 +3687,7 @@
       <c r="F70" t="s">
         <v>24</v>
       </c>
-      <c r="G70" t="s">
+      <c r="G70" s="5" t="s">
         <v>160</v>
       </c>
       <c r="H70" t="s">
@@ -3682,26 +3696,26 @@
       <c r="I70" t="s">
         <v>82</v>
       </c>
-      <c r="J70" s="7"/>
-      <c r="K70" s="7"/>
-      <c r="L70" s="7"/>
-      <c r="M70" s="7"/>
-      <c r="N70" s="7"/>
-      <c r="O70" s="7"/>
-      <c r="P70" s="7"/>
-      <c r="Q70" s="7"/>
-      <c r="R70" s="7"/>
-      <c r="S70" s="7"/>
-      <c r="T70" s="7"/>
-    </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A71" s="6">
+      <c r="J70" s="3"/>
+      <c r="K70" s="3"/>
+      <c r="L70" s="3"/>
+      <c r="M70" s="3"/>
+      <c r="N70" s="3"/>
+      <c r="O70" s="3"/>
+      <c r="P70" s="3"/>
+      <c r="Q70" s="3"/>
+      <c r="R70" s="3"/>
+      <c r="S70" s="3"/>
+      <c r="T70" s="3"/>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A71" s="2">
         <v>70</v>
       </c>
       <c r="B71" t="s">
         <v>75</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C71" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D71" t="s">
@@ -3713,7 +3727,7 @@
       <c r="F71" t="s">
         <v>24</v>
       </c>
-      <c r="G71" t="s">
+      <c r="G71" s="5" t="s">
         <v>76</v>
       </c>
       <c r="H71" t="s">
@@ -3722,26 +3736,26 @@
       <c r="I71" t="s">
         <v>82</v>
       </c>
-      <c r="J71" s="7"/>
-      <c r="K71" s="7"/>
-      <c r="L71" s="7"/>
-      <c r="M71" s="7"/>
-      <c r="N71" s="7"/>
-      <c r="O71" s="7"/>
-      <c r="P71" s="7"/>
-      <c r="Q71" s="7"/>
-      <c r="R71" s="7"/>
-      <c r="S71" s="7"/>
-      <c r="T71" s="7"/>
-    </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A72" s="6">
+      <c r="J71" s="3"/>
+      <c r="K71" s="3"/>
+      <c r="L71" s="3"/>
+      <c r="M71" s="3"/>
+      <c r="N71" s="3"/>
+      <c r="O71" s="3"/>
+      <c r="P71" s="3"/>
+      <c r="Q71" s="3"/>
+      <c r="R71" s="3"/>
+      <c r="S71" s="3"/>
+      <c r="T71" s="3"/>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A72" s="2">
         <v>71</v>
       </c>
       <c r="B72" t="s">
         <v>77</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C72" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D72" t="s">
@@ -3753,7 +3767,7 @@
       <c r="F72" t="s">
         <v>15</v>
       </c>
-      <c r="G72" t="s">
+      <c r="G72" s="5" t="s">
         <v>76</v>
       </c>
       <c r="H72" t="s">
@@ -3762,26 +3776,26 @@
       <c r="I72" t="s">
         <v>82</v>
       </c>
-      <c r="J72" s="7"/>
-      <c r="K72" s="7"/>
-      <c r="L72" s="7"/>
-      <c r="M72" s="7"/>
-      <c r="N72" s="7"/>
-      <c r="O72" s="7"/>
-      <c r="P72" s="7"/>
-      <c r="Q72" s="7"/>
-      <c r="R72" s="7"/>
-      <c r="S72" s="7"/>
-      <c r="T72" s="7"/>
-    </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A73" s="6">
+      <c r="J72" s="3"/>
+      <c r="K72" s="3"/>
+      <c r="L72" s="3"/>
+      <c r="M72" s="3"/>
+      <c r="N72" s="3"/>
+      <c r="O72" s="3"/>
+      <c r="P72" s="3"/>
+      <c r="Q72" s="3"/>
+      <c r="R72" s="3"/>
+      <c r="S72" s="3"/>
+      <c r="T72" s="3"/>
+    </row>
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A73" s="2">
         <v>72</v>
       </c>
       <c r="B73" t="s">
         <v>78</v>
       </c>
-      <c r="C73" s="5" t="s">
+      <c r="C73" s="6" t="s">
         <v>145</v>
       </c>
       <c r="D73" t="s">
@@ -3793,7 +3807,7 @@
       <c r="F73" t="s">
         <v>28</v>
       </c>
-      <c r="G73" t="s">
+      <c r="G73" s="5" t="s">
         <v>76</v>
       </c>
       <c r="H73" t="s">
@@ -3802,26 +3816,26 @@
       <c r="I73" t="s">
         <v>82</v>
       </c>
-      <c r="J73" s="7"/>
-      <c r="K73" s="7"/>
-      <c r="L73" s="7"/>
-      <c r="M73" s="7"/>
-      <c r="N73" s="7"/>
-      <c r="O73" s="7"/>
-      <c r="P73" s="7"/>
-      <c r="Q73" s="7"/>
-      <c r="R73" s="7"/>
-      <c r="S73" s="7"/>
-      <c r="T73" s="7"/>
-    </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A74" s="6">
+      <c r="J73" s="3"/>
+      <c r="K73" s="3"/>
+      <c r="L73" s="3"/>
+      <c r="M73" s="3"/>
+      <c r="N73" s="3"/>
+      <c r="O73" s="3"/>
+      <c r="P73" s="3"/>
+      <c r="Q73" s="3"/>
+      <c r="R73" s="3"/>
+      <c r="S73" s="3"/>
+      <c r="T73" s="3"/>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A74" s="2">
         <v>73</v>
       </c>
       <c r="B74" t="s">
         <v>79</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74" s="5" t="s">
         <v>146</v>
       </c>
       <c r="D74" t="s">
@@ -3833,8 +3847,8 @@
       <c r="F74" t="s">
         <v>155</v>
       </c>
-      <c r="G74">
-        <v>57</v>
+      <c r="G74" s="5" t="s">
+        <v>76</v>
       </c>
       <c r="H74" t="s">
         <v>165</v>
@@ -3842,26 +3856,26 @@
       <c r="I74" t="s">
         <v>82</v>
       </c>
-      <c r="J74" s="7"/>
-      <c r="K74" s="7"/>
-      <c r="L74" s="7"/>
-      <c r="M74" s="7"/>
-      <c r="N74" s="7"/>
-      <c r="O74" s="7"/>
-      <c r="P74" s="7"/>
-      <c r="Q74" s="7"/>
-      <c r="R74" s="7"/>
-      <c r="S74" s="7"/>
-      <c r="T74" s="7"/>
-    </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A75" s="6">
+      <c r="J74" s="3"/>
+      <c r="K74" s="3"/>
+      <c r="L74" s="3"/>
+      <c r="M74" s="3"/>
+      <c r="N74" s="3"/>
+      <c r="O74" s="3"/>
+      <c r="P74" s="3"/>
+      <c r="Q74" s="3"/>
+      <c r="R74" s="3"/>
+      <c r="S74" s="3"/>
+      <c r="T74" s="3"/>
+    </row>
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A75" s="2">
         <v>74</v>
       </c>
       <c r="B75" t="s">
         <v>80</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C75" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D75" t="s">
@@ -3873,7 +3887,7 @@
       <c r="F75" t="s">
         <v>9</v>
       </c>
-      <c r="G75" t="s">
+      <c r="G75" s="5" t="s">
         <v>81</v>
       </c>
       <c r="H75" t="s">
@@ -3882,26 +3896,26 @@
       <c r="I75" t="s">
         <v>82</v>
       </c>
-      <c r="J75" s="7"/>
-      <c r="K75" s="7"/>
-      <c r="L75" s="7"/>
-      <c r="M75" s="7"/>
-      <c r="N75" s="7"/>
-      <c r="O75" s="7"/>
-      <c r="P75" s="7"/>
-      <c r="Q75" s="7"/>
-      <c r="R75" s="7"/>
-      <c r="S75" s="7"/>
-      <c r="T75" s="7"/>
-    </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A76" s="6">
+      <c r="J75" s="3"/>
+      <c r="K75" s="3"/>
+      <c r="L75" s="3"/>
+      <c r="M75" s="3"/>
+      <c r="N75" s="3"/>
+      <c r="O75" s="3"/>
+      <c r="P75" s="3"/>
+      <c r="Q75" s="3"/>
+      <c r="R75" s="3"/>
+      <c r="S75" s="3"/>
+      <c r="T75" s="3"/>
+    </row>
+    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A76" s="2">
         <v>75</v>
       </c>
       <c r="B76" t="s">
         <v>126</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C76" s="5" t="s">
         <v>83</v>
       </c>
       <c r="D76" t="s">
@@ -3913,7 +3927,7 @@
       <c r="F76" t="s">
         <v>57</v>
       </c>
-      <c r="G76" t="s">
+      <c r="G76" s="5" t="s">
         <v>81</v>
       </c>
       <c r="H76" t="s">
@@ -3922,26 +3936,26 @@
       <c r="I76" t="s">
         <v>82</v>
       </c>
-      <c r="J76" s="7"/>
-      <c r="K76" s="7"/>
-      <c r="L76" s="7"/>
-      <c r="M76" s="7"/>
-      <c r="N76" s="7"/>
-      <c r="O76" s="7"/>
-      <c r="P76" s="7"/>
-      <c r="Q76" s="7"/>
-      <c r="R76" s="7"/>
-      <c r="S76" s="7"/>
-      <c r="T76" s="7"/>
-    </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A77" s="6">
+      <c r="J76" s="3"/>
+      <c r="K76" s="3"/>
+      <c r="L76" s="3"/>
+      <c r="M76" s="3"/>
+      <c r="N76" s="3"/>
+      <c r="O76" s="3"/>
+      <c r="P76" s="3"/>
+      <c r="Q76" s="3"/>
+      <c r="R76" s="3"/>
+      <c r="S76" s="3"/>
+      <c r="T76" s="3"/>
+    </row>
+    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A77" s="2">
         <v>76</v>
       </c>
       <c r="B77" t="s">
         <v>127</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C77" s="5" t="s">
         <v>57</v>
       </c>
       <c r="D77" t="s">
@@ -3953,7 +3967,7 @@
       <c r="F77" t="s">
         <v>57</v>
       </c>
-      <c r="G77" t="s">
+      <c r="G77" s="5" t="s">
         <v>81</v>
       </c>
       <c r="H77" t="s">
@@ -3962,26 +3976,26 @@
       <c r="I77" t="s">
         <v>82</v>
       </c>
-      <c r="J77" s="7"/>
-      <c r="K77" s="7"/>
-      <c r="L77" s="7"/>
-      <c r="M77" s="7"/>
-      <c r="N77" s="7"/>
-      <c r="O77" s="7"/>
-      <c r="P77" s="7"/>
-      <c r="Q77" s="7"/>
-      <c r="R77" s="7"/>
-      <c r="S77" s="7"/>
-      <c r="T77" s="7"/>
-    </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A78" s="6">
+      <c r="J77" s="3"/>
+      <c r="K77" s="3"/>
+      <c r="L77" s="3"/>
+      <c r="M77" s="3"/>
+      <c r="N77" s="3"/>
+      <c r="O77" s="3"/>
+      <c r="P77" s="3"/>
+      <c r="Q77" s="3"/>
+      <c r="R77" s="3"/>
+      <c r="S77" s="3"/>
+      <c r="T77" s="3"/>
+    </row>
+    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A78" s="2">
         <v>77</v>
       </c>
       <c r="B78" t="s">
         <v>128</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C78" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D78" t="s">
@@ -3993,7 +4007,7 @@
       <c r="F78" t="s">
         <v>9</v>
       </c>
-      <c r="G78" t="s">
+      <c r="G78" s="5" t="s">
         <v>84</v>
       </c>
       <c r="H78" t="s">
@@ -4002,26 +4016,26 @@
       <c r="I78" t="s">
         <v>82</v>
       </c>
-      <c r="J78" s="7"/>
-      <c r="K78" s="7"/>
-      <c r="L78" s="7"/>
-      <c r="M78" s="7"/>
-      <c r="N78" s="7"/>
-      <c r="O78" s="7"/>
-      <c r="P78" s="7"/>
-      <c r="Q78" s="7"/>
-      <c r="R78" s="7"/>
-      <c r="S78" s="7"/>
-      <c r="T78" s="7"/>
-    </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A79" s="6">
+      <c r="J78" s="3"/>
+      <c r="K78" s="3"/>
+      <c r="L78" s="3"/>
+      <c r="M78" s="3"/>
+      <c r="N78" s="3"/>
+      <c r="O78" s="3"/>
+      <c r="P78" s="3"/>
+      <c r="Q78" s="3"/>
+      <c r="R78" s="3"/>
+      <c r="S78" s="3"/>
+      <c r="T78" s="3"/>
+    </row>
+    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A79" s="2">
         <v>78</v>
       </c>
       <c r="B79" t="s">
         <v>85</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C79" s="5" t="s">
         <v>36</v>
       </c>
       <c r="D79" t="s">
@@ -4033,7 +4047,7 @@
       <c r="F79" t="s">
         <v>15</v>
       </c>
-      <c r="G79" t="s">
+      <c r="G79" s="5" t="s">
         <v>84</v>
       </c>
       <c r="H79" t="s">
@@ -4042,26 +4056,26 @@
       <c r="I79" t="s">
         <v>82</v>
       </c>
-      <c r="J79" s="7"/>
-      <c r="K79" s="7"/>
-      <c r="L79" s="7"/>
-      <c r="M79" s="7"/>
-      <c r="N79" s="7"/>
-      <c r="O79" s="7"/>
-      <c r="P79" s="7"/>
-      <c r="Q79" s="7"/>
-      <c r="R79" s="7"/>
-      <c r="S79" s="7"/>
-      <c r="T79" s="7"/>
-    </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A80" s="6">
+      <c r="J79" s="3"/>
+      <c r="K79" s="3"/>
+      <c r="L79" s="3"/>
+      <c r="M79" s="3"/>
+      <c r="N79" s="3"/>
+      <c r="O79" s="3"/>
+      <c r="P79" s="3"/>
+      <c r="Q79" s="3"/>
+      <c r="R79" s="3"/>
+      <c r="S79" s="3"/>
+      <c r="T79" s="3"/>
+    </row>
+    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A80" s="2">
         <v>79</v>
       </c>
       <c r="B80" t="s">
         <v>86</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C80" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D80" t="s">
@@ -4073,7 +4087,7 @@
       <c r="F80" t="s">
         <v>15</v>
       </c>
-      <c r="G80" t="s">
+      <c r="G80" s="5" t="s">
         <v>84</v>
       </c>
       <c r="H80" t="s">
@@ -4082,62 +4096,34 @@
       <c r="I80" t="s">
         <v>82</v>
       </c>
-      <c r="J80" s="7"/>
-      <c r="K80" s="7"/>
-      <c r="L80" s="7"/>
-      <c r="M80" s="7"/>
-      <c r="N80" s="7"/>
-      <c r="O80" s="7"/>
-      <c r="P80" s="7"/>
-      <c r="Q80" s="7"/>
-      <c r="R80" s="7"/>
-      <c r="S80" s="7"/>
-      <c r="T80" s="7"/>
-    </row>
-    <row r="81" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J81" s="7"/>
-      <c r="K81" s="7"/>
-      <c r="L81" s="7"/>
-      <c r="M81" s="7"/>
-      <c r="N81" s="7"/>
-      <c r="O81" s="7"/>
-      <c r="P81" s="7"/>
-      <c r="Q81" s="7"/>
-      <c r="R81" s="7"/>
-      <c r="S81" s="7"/>
-      <c r="T81" s="7"/>
+      <c r="J80" s="3"/>
+      <c r="K80" s="3"/>
+      <c r="L80" s="3"/>
+      <c r="M80" s="3"/>
+      <c r="N80" s="3"/>
+      <c r="O80" s="3"/>
+      <c r="P80" s="3"/>
+      <c r="Q80" s="3"/>
+      <c r="R80" s="3"/>
+      <c r="S80" s="3"/>
+      <c r="T80" s="3"/>
+    </row>
+    <row r="81" spans="10:20" x14ac:dyDescent="0.25">
+      <c r="J81" s="3"/>
+      <c r="K81" s="3"/>
+      <c r="L81" s="3"/>
+      <c r="M81" s="3"/>
+      <c r="N81" s="3"/>
+      <c r="O81" s="3"/>
+      <c r="P81" s="3"/>
+      <c r="Q81" s="3"/>
+      <c r="R81" s="3"/>
+      <c r="S81" s="3"/>
+      <c r="T81" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <phoneticPr fontId="0" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter alignWithMargins="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <phoneticPr fontId="0" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter alignWithMargins="0"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Identified datafiles for update
</commit_message>
<xml_diff>
--- a/Attributes.xlsx
+++ b/Attributes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\Documents\Visual Studio 2019\Projects\BESM3CA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908D9E43-F827-4039-8B1A-2D9C4362E1A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C522D9DF-DF7F-4070-8EE8-E97D75F9CFB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8640" yWindow="4740" windowWidth="28800" windowHeight="15470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="173">
   <si>
     <t>Attribute Name</t>
   </si>
@@ -536,6 +536,9 @@
   </si>
   <si>
     <t>44</t>
+  </si>
+  <si>
+    <t>Description</t>
   </si>
 </sst>
 </file>
@@ -901,7 +904,7 @@
   <dimension ref="A1:T81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -912,7 +915,7 @@
     <col min="5" max="7" width="22.453125" customWidth="1"/>
     <col min="8" max="8" width="7.08984375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.6328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.81640625" customWidth="1"/>
     <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
@@ -944,7 +947,9 @@
       <c r="I1" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="J1" s="1"/>
+      <c r="J1" s="1" t="s">
+        <v>172</v>
+      </c>
       <c r="K1" s="1"/>
       <c r="M1" s="1"/>
     </row>

</xml_diff>

<commit_message>
Added initial description calculations Fixed errors with companion and item points calculations
</commit_message>
<xml_diff>
--- a/Attributes.xlsx
+++ b/Attributes.xlsx
@@ -8,19 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\Documents\Visual Studio 2019\Projects\BESM3CA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C522D9DF-DF7F-4070-8EE8-E97D75F9CFB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E46C9376-B3C3-47BD-8552-9C00C2AA81D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8640" yWindow="4740" windowWidth="28800" windowHeight="15470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26565" yWindow="375" windowWidth="25725" windowHeight="14910" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Attributes" sheetId="1" r:id="rId1"/>
+    <sheet name="Progressions" sheetId="4" r:id="rId2"/>
+    <sheet name="Special" sheetId="2" r:id="rId3"/>
+    <sheet name="Variables" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="92512"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Attributes!$A$1:$J$82</definedName>
+  </definedNames>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="242">
   <si>
     <t>Attribute Name</t>
   </si>
@@ -539,19 +545,231 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>Ageing</t>
+  </si>
+  <si>
+    <t>Balance</t>
+  </si>
+  <si>
+    <t>Blind Fighting</t>
+  </si>
+  <si>
+    <t>Blind Shooting</t>
+  </si>
+  <si>
+    <t>Brutal</t>
+  </si>
+  <si>
+    <t>Cat-Like</t>
+  </si>
+  <si>
+    <t>Concealment</t>
+  </si>
+  <si>
+    <t>Critical Strike</t>
+  </si>
+  <si>
+    <t>Dead Eye</t>
+  </si>
+  <si>
+    <t>Deflection</t>
+  </si>
+  <si>
+    <t>Disease</t>
+  </si>
+  <si>
+    <t>Extended Range</t>
+  </si>
+  <si>
+    <t>Far Shot</t>
+  </si>
+  <si>
+    <t>Flare Variable</t>
+  </si>
+  <si>
+    <t>Freezing Cold</t>
+  </si>
+  <si>
+    <t>Freezing Water</t>
+  </si>
+  <si>
+    <t>Hardboiled</t>
+  </si>
+  <si>
+    <t>High Pressure</t>
+  </si>
+  <si>
+    <t>Judge Opponent</t>
+  </si>
+  <si>
+    <t>Lack of Air</t>
+  </si>
+  <si>
+    <t>Lack of Food</t>
+  </si>
+  <si>
+    <t>Lack of Water</t>
+  </si>
+  <si>
+    <t>Leap Attack</t>
+  </si>
+  <si>
+    <t>Lethal Blow</t>
+  </si>
+  <si>
+    <t>Light-Footed</t>
+  </si>
+  <si>
+    <t>Lightning Reflexes</t>
+  </si>
+  <si>
+    <t>Low Pressure</t>
+  </si>
+  <si>
+    <t>Multiple Targets</t>
+  </si>
+  <si>
+    <t>Overheating</t>
+  </si>
+  <si>
+    <t>Poison</t>
+  </si>
+  <si>
+    <t>Portable Armoury</t>
+  </si>
+  <si>
+    <t>Precise Aim</t>
+  </si>
+  <si>
+    <t>Reflection</t>
+  </si>
+  <si>
+    <t>Sleep</t>
+  </si>
+  <si>
+    <t>Slithering</t>
+  </si>
+  <si>
+    <t>Specific Weapon Variable</t>
+  </si>
+  <si>
+    <t>Steady Hand</t>
+  </si>
+  <si>
+    <t>Swinging / Brachiating</t>
+  </si>
+  <si>
+    <t>Tournament Encyclopaedia</t>
+  </si>
+  <si>
+    <t>Two Weapons</t>
+  </si>
+  <si>
+    <t>Untrackable</t>
+  </si>
+  <si>
+    <t>Wall-Bouncing</t>
+  </si>
+  <si>
+    <t>Wall-Crawling</t>
+  </si>
+  <si>
+    <t>Water-Walking</t>
+  </si>
+  <si>
+    <t>Weapons Encyclopaedia</t>
+  </si>
+  <si>
+    <t>Zen Direction</t>
+  </si>
+  <si>
+    <t>Accurate</t>
+  </si>
+  <si>
+    <t>Astral Projection</t>
+  </si>
+  <si>
+    <t>Missing</t>
+  </si>
+  <si>
+    <t>Rank</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Permanent</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1 round</t>
+  </si>
+  <si>
+    <t>5 round</t>
+  </si>
+  <si>
+    <t>1 minute</t>
+  </si>
+  <si>
+    <t>10 minutes</t>
+  </si>
+  <si>
+    <t>1 hour</t>
+  </si>
+  <si>
+    <t>4 hours</t>
+  </si>
+  <si>
+    <t>12 hours</t>
+  </si>
+  <si>
+    <t>1 day</t>
+  </si>
+  <si>
+    <t>1 week</t>
+  </si>
+  <si>
+    <t>1 month</t>
+  </si>
+  <si>
+    <t>1 season</t>
+  </si>
+  <si>
+    <t>1 year</t>
+  </si>
+  <si>
+    <t>10 years</t>
+  </si>
+  <si>
+    <t>100 years</t>
+  </si>
+  <si>
+    <t>1000 years</t>
+  </si>
+  <si>
+    <t>"100,000,000,000,000","1,000,000,000,000,000",</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -577,7 +795,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -587,6 +805,8 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -901,10 +1121,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T81"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:T82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1553,7 +1774,7 @@
       <c r="S16" s="3"/>
       <c r="T16" s="3"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1581,7 +1802,9 @@
       <c r="I17" t="s">
         <v>82</v>
       </c>
-      <c r="J17" s="3"/>
+      <c r="J17" s="3" t="s">
+        <v>221</v>
+      </c>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
@@ -1753,7 +1976,7 @@
       <c r="S21" s="3"/>
       <c r="T21" s="3"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1781,7 +2004,9 @@
       <c r="I22" t="s">
         <v>82</v>
       </c>
-      <c r="J22" s="3"/>
+      <c r="J22" s="3" t="s">
+        <v>221</v>
+      </c>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
@@ -2193,7 +2418,7 @@
       <c r="S32" s="3"/>
       <c r="T32" s="3"/>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -2221,7 +2446,9 @@
       <c r="I33" t="s">
         <v>82</v>
       </c>
-      <c r="J33" s="3"/>
+      <c r="J33" s="3" t="s">
+        <v>221</v>
+      </c>
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
@@ -2273,7 +2500,7 @@
       <c r="S34" s="3"/>
       <c r="T34" s="3"/>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -2301,7 +2528,9 @@
       <c r="I35" t="s">
         <v>82</v>
       </c>
-      <c r="J35" s="3"/>
+      <c r="J35" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
@@ -2593,7 +2822,7 @@
       <c r="S42" s="3"/>
       <c r="T42" s="3"/>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -2621,7 +2850,9 @@
       <c r="I43" t="s">
         <v>82</v>
       </c>
-      <c r="J43" s="3"/>
+      <c r="J43" s="3" t="s">
+        <v>221</v>
+      </c>
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
@@ -2713,7 +2944,7 @@
       <c r="S45" s="3"/>
       <c r="T45" s="3"/>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -2741,7 +2972,9 @@
       <c r="I46" t="s">
         <v>82</v>
       </c>
-      <c r="J46" s="3"/>
+      <c r="J46" s="3" t="s">
+        <v>221</v>
+      </c>
       <c r="K46" s="3"/>
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
@@ -3273,7 +3506,7 @@
       <c r="S59" s="3"/>
       <c r="T59" s="3"/>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -3301,7 +3534,9 @@
       <c r="I60" t="s">
         <v>82</v>
       </c>
-      <c r="J60" s="3"/>
+      <c r="J60" s="3" t="s">
+        <v>221</v>
+      </c>
       <c r="K60" s="3"/>
       <c r="L60" s="3"/>
       <c r="M60" s="3"/>
@@ -3353,7 +3588,7 @@
       <c r="S61" s="3"/>
       <c r="T61" s="3"/>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -3381,7 +3616,9 @@
       <c r="I62" t="s">
         <v>82</v>
       </c>
-      <c r="J62" s="3"/>
+      <c r="J62" s="3" t="s">
+        <v>221</v>
+      </c>
       <c r="K62" s="3"/>
       <c r="L62" s="3"/>
       <c r="M62" s="3"/>
@@ -3393,7 +3630,7 @@
       <c r="S62" s="3"/>
       <c r="T62" s="3"/>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -3421,7 +3658,9 @@
       <c r="I63" t="s">
         <v>82</v>
       </c>
-      <c r="J63" s="3"/>
+      <c r="J63" s="3" t="s">
+        <v>221</v>
+      </c>
       <c r="K63" s="3"/>
       <c r="L63" s="3"/>
       <c r="M63" s="3"/>
@@ -3433,7 +3672,7 @@
       <c r="S63" s="3"/>
       <c r="T63" s="3"/>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -3461,7 +3700,9 @@
       <c r="I64" t="s">
         <v>82</v>
       </c>
-      <c r="J64" s="3"/>
+      <c r="J64" s="3" t="s">
+        <v>221</v>
+      </c>
       <c r="K64" s="3"/>
       <c r="L64" s="3"/>
       <c r="M64" s="3"/>
@@ -3473,7 +3714,7 @@
       <c r="S64" s="3"/>
       <c r="T64" s="3"/>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -3501,7 +3742,9 @@
       <c r="I65" t="s">
         <v>82</v>
       </c>
-      <c r="J65" s="3"/>
+      <c r="J65" s="3" t="s">
+        <v>221</v>
+      </c>
       <c r="K65" s="3"/>
       <c r="L65" s="3"/>
       <c r="M65" s="3"/>
@@ -3513,7 +3756,7 @@
       <c r="S65" s="3"/>
       <c r="T65" s="3"/>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -3541,7 +3784,9 @@
       <c r="I66" t="s">
         <v>82</v>
       </c>
-      <c r="J66" s="3"/>
+      <c r="J66" s="3" t="s">
+        <v>221</v>
+      </c>
       <c r="K66" s="3"/>
       <c r="L66" s="3"/>
       <c r="M66" s="3"/>
@@ -3553,7 +3798,7 @@
       <c r="S66" s="3"/>
       <c r="T66" s="3"/>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -3581,7 +3826,9 @@
       <c r="I67" t="s">
         <v>82</v>
       </c>
-      <c r="J67" s="3"/>
+      <c r="J67" s="3" t="s">
+        <v>221</v>
+      </c>
       <c r="K67" s="3"/>
       <c r="L67" s="3"/>
       <c r="M67" s="3"/>
@@ -3593,7 +3840,7 @@
       <c r="S67" s="3"/>
       <c r="T67" s="3"/>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -3621,7 +3868,9 @@
       <c r="I68" t="s">
         <v>82</v>
       </c>
-      <c r="J68" s="3"/>
+      <c r="J68" s="3" t="s">
+        <v>221</v>
+      </c>
       <c r="K68" s="3"/>
       <c r="L68" s="3"/>
       <c r="M68" s="3"/>
@@ -3633,7 +3882,7 @@
       <c r="S68" s="3"/>
       <c r="T68" s="3"/>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>68</v>
       </c>
@@ -3661,7 +3910,9 @@
       <c r="I69" t="s">
         <v>82</v>
       </c>
-      <c r="J69" s="3"/>
+      <c r="J69" s="3" t="s">
+        <v>221</v>
+      </c>
       <c r="K69" s="3"/>
       <c r="L69" s="3"/>
       <c r="M69" s="3"/>
@@ -3673,7 +3924,7 @@
       <c r="S69" s="3"/>
       <c r="T69" s="3"/>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>69</v>
       </c>
@@ -3701,7 +3952,9 @@
       <c r="I70" t="s">
         <v>82</v>
       </c>
-      <c r="J70" s="3"/>
+      <c r="J70" s="3" t="s">
+        <v>221</v>
+      </c>
       <c r="K70" s="3"/>
       <c r="L70" s="3"/>
       <c r="M70" s="3"/>
@@ -3713,7 +3966,7 @@
       <c r="S70" s="3"/>
       <c r="T70" s="3"/>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>70</v>
       </c>
@@ -3741,7 +3994,9 @@
       <c r="I71" t="s">
         <v>82</v>
       </c>
-      <c r="J71" s="3"/>
+      <c r="J71" s="3" t="s">
+        <v>221</v>
+      </c>
       <c r="K71" s="3"/>
       <c r="L71" s="3"/>
       <c r="M71" s="3"/>
@@ -3753,7 +4008,7 @@
       <c r="S71" s="3"/>
       <c r="T71" s="3"/>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>71</v>
       </c>
@@ -3781,7 +4036,9 @@
       <c r="I72" t="s">
         <v>82</v>
       </c>
-      <c r="J72" s="3"/>
+      <c r="J72" s="3" t="s">
+        <v>221</v>
+      </c>
       <c r="K72" s="3"/>
       <c r="L72" s="3"/>
       <c r="M72" s="3"/>
@@ -3793,7 +4050,7 @@
       <c r="S72" s="3"/>
       <c r="T72" s="3"/>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>72</v>
       </c>
@@ -3821,7 +4078,9 @@
       <c r="I73" t="s">
         <v>82</v>
       </c>
-      <c r="J73" s="3"/>
+      <c r="J73" s="3" t="s">
+        <v>221</v>
+      </c>
       <c r="K73" s="3"/>
       <c r="L73" s="3"/>
       <c r="M73" s="3"/>
@@ -3833,7 +4092,7 @@
       <c r="S73" s="3"/>
       <c r="T73" s="3"/>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>73</v>
       </c>
@@ -3861,7 +4120,9 @@
       <c r="I74" t="s">
         <v>82</v>
       </c>
-      <c r="J74" s="3"/>
+      <c r="J74" s="3" t="s">
+        <v>221</v>
+      </c>
       <c r="K74" s="3"/>
       <c r="L74" s="3"/>
       <c r="M74" s="3"/>
@@ -3873,7 +4134,7 @@
       <c r="S74" s="3"/>
       <c r="T74" s="3"/>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>74</v>
       </c>
@@ -3901,7 +4162,9 @@
       <c r="I75" t="s">
         <v>82</v>
       </c>
-      <c r="J75" s="3"/>
+      <c r="J75" s="3" t="s">
+        <v>221</v>
+      </c>
       <c r="K75" s="3"/>
       <c r="L75" s="3"/>
       <c r="M75" s="3"/>
@@ -3913,7 +4176,7 @@
       <c r="S75" s="3"/>
       <c r="T75" s="3"/>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>75</v>
       </c>
@@ -3941,7 +4204,9 @@
       <c r="I76" t="s">
         <v>82</v>
       </c>
-      <c r="J76" s="3"/>
+      <c r="J76" s="3" t="s">
+        <v>221</v>
+      </c>
       <c r="K76" s="3"/>
       <c r="L76" s="3"/>
       <c r="M76" s="3"/>
@@ -3993,7 +4258,7 @@
       <c r="S77" s="3"/>
       <c r="T77" s="3"/>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>77</v>
       </c>
@@ -4021,7 +4286,9 @@
       <c r="I78" t="s">
         <v>82</v>
       </c>
-      <c r="J78" s="3"/>
+      <c r="J78" s="3" t="s">
+        <v>221</v>
+      </c>
       <c r="K78" s="3"/>
       <c r="L78" s="3"/>
       <c r="M78" s="3"/>
@@ -4033,7 +4300,7 @@
       <c r="S78" s="3"/>
       <c r="T78" s="3"/>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>78</v>
       </c>
@@ -4061,7 +4328,9 @@
       <c r="I79" t="s">
         <v>82</v>
       </c>
-      <c r="J79" s="3"/>
+      <c r="J79" s="3" t="s">
+        <v>221</v>
+      </c>
       <c r="K79" s="3"/>
       <c r="L79" s="3"/>
       <c r="M79" s="3"/>
@@ -4073,7 +4342,7 @@
       <c r="S79" s="3"/>
       <c r="T79" s="3"/>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>79</v>
       </c>
@@ -4101,7 +4370,9 @@
       <c r="I80" t="s">
         <v>82</v>
       </c>
-      <c r="J80" s="3"/>
+      <c r="J80" s="3" t="s">
+        <v>221</v>
+      </c>
       <c r="K80" s="3"/>
       <c r="L80" s="3"/>
       <c r="M80" s="3"/>
@@ -4113,8 +4384,13 @@
       <c r="S80" s="3"/>
       <c r="T80" s="3"/>
     </row>
-    <row r="81" spans="10:20" x14ac:dyDescent="0.25">
-      <c r="J81" s="3"/>
+    <row r="81" spans="2:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>220</v>
+      </c>
+      <c r="J81" s="3" t="s">
+        <v>221</v>
+      </c>
       <c r="K81" s="3"/>
       <c r="L81" s="3"/>
       <c r="M81" s="3"/>
@@ -4126,9 +4402,1209 @@
       <c r="S81" s="3"/>
       <c r="T81" s="3"/>
     </row>
+    <row r="82" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="J82" s="3"/>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:J82" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="9">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2682129-B781-437F-82ED-9C9C70CEE7CF}">
+  <dimension ref="A1:P20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.7265625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.54296875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="36" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.90625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="10" width="10.90625" style="7" customWidth="1"/>
+    <col min="11" max="11" width="6.36328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="6.36328125" style="7" customWidth="1"/>
+    <col min="14" max="14" width="9.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1"/>
+      <c r="D1"/>
+      <c r="E1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1"/>
+      <c r="G1"/>
+      <c r="H1"/>
+      <c r="I1"/>
+      <c r="J1"/>
+      <c r="K1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1"/>
+      <c r="M1"/>
+      <c r="N1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7">
+        <v>0</v>
+      </c>
+      <c r="C2" s="7" t="str">
+        <f>""""&amp;TEXT(B2,"#,##0")&amp;""","</f>
+        <v>"0",</v>
+      </c>
+      <c r="D2" s="7" t="str">
+        <f>C2</f>
+        <v>"0",</v>
+      </c>
+      <c r="E2" s="7">
+        <v>0</v>
+      </c>
+      <c r="F2" s="7" t="str">
+        <f>""""&amp;TEXT(E2,"#,##0")&amp;""","</f>
+        <v>"0",</v>
+      </c>
+      <c r="G2" s="7" t="str">
+        <f>F2</f>
+        <v>"0",</v>
+      </c>
+      <c r="K2" s="7">
+        <v>0</v>
+      </c>
+      <c r="L2" s="7" t="str">
+        <f>""""&amp;TEXT(K2,"#,##0")&amp;""","</f>
+        <v>"0",</v>
+      </c>
+      <c r="M2" s="7" t="str">
+        <f>L2</f>
+        <v>"0",</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="O2" s="7" t="str">
+        <f>""""&amp;N2&amp;""","</f>
+        <v>"0",</v>
+      </c>
+      <c r="P2" s="7" t="str">
+        <f>O2</f>
+        <v>"0",</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7" t="str">
+        <f t="shared" ref="C3:C18" si="0">""""&amp;TEXT(B3,"#,##0")&amp;""","</f>
+        <v>"1",</v>
+      </c>
+      <c r="D3" s="7" t="str">
+        <f>D2&amp;C3</f>
+        <v>"0","1",</v>
+      </c>
+      <c r="E3" s="7">
+        <v>1</v>
+      </c>
+      <c r="F3" s="7" t="str">
+        <f t="shared" ref="F3:F18" si="1">""""&amp;TEXT(E3,"#,##0")&amp;""","</f>
+        <v>"1",</v>
+      </c>
+      <c r="G3" s="7" t="str">
+        <f>G2&amp;F3</f>
+        <v>"0","1",</v>
+      </c>
+      <c r="K3" s="7">
+        <v>1</v>
+      </c>
+      <c r="L3" s="7" t="str">
+        <f t="shared" ref="L3:L18" si="2">""""&amp;TEXT(K3,"#,##0")&amp;""","</f>
+        <v>"1",</v>
+      </c>
+      <c r="M3" s="7" t="str">
+        <f>M2&amp;L3</f>
+        <v>"0","1",</v>
+      </c>
+      <c r="N3" t="s">
+        <v>226</v>
+      </c>
+      <c r="O3" s="7" t="str">
+        <f t="shared" ref="O3:O18" si="3">""""&amp;N3&amp;""","</f>
+        <v>"1 round",</v>
+      </c>
+      <c r="P3" s="7" t="str">
+        <f>P2&amp;O3</f>
+        <v>"0","1 round",</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7">
+        <v>10</v>
+      </c>
+      <c r="C4" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>"10",</v>
+      </c>
+      <c r="D4" s="7" t="str">
+        <f t="shared" ref="D4:D18" si="4">D3&amp;C4</f>
+        <v>"0","1","10",</v>
+      </c>
+      <c r="E4" s="7">
+        <v>3</v>
+      </c>
+      <c r="F4" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>"3",</v>
+      </c>
+      <c r="G4" s="7" t="str">
+        <f t="shared" ref="G4:G18" si="5">G3&amp;F4</f>
+        <v>"0","1","3",</v>
+      </c>
+      <c r="K4" s="7">
+        <v>2</v>
+      </c>
+      <c r="L4" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>"2",</v>
+      </c>
+      <c r="M4" s="7" t="str">
+        <f t="shared" ref="M4:M18" si="6">M3&amp;L4</f>
+        <v>"0","1","2",</v>
+      </c>
+      <c r="N4" t="s">
+        <v>227</v>
+      </c>
+      <c r="O4" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>"5 round",</v>
+      </c>
+      <c r="P4" s="7" t="str">
+        <f t="shared" ref="P4:P18" si="7">P3&amp;O4</f>
+        <v>"0","1 round","5 round",</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="7">
+        <v>100</v>
+      </c>
+      <c r="C5" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>"100",</v>
+      </c>
+      <c r="D5" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v>"0","1","10","100",</v>
+      </c>
+      <c r="E5" s="7">
+        <v>10</v>
+      </c>
+      <c r="F5" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>"10",</v>
+      </c>
+      <c r="G5" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>"0","1","3","10",</v>
+      </c>
+      <c r="K5" s="7">
+        <v>4</v>
+      </c>
+      <c r="L5" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>"4",</v>
+      </c>
+      <c r="M5" s="7" t="str">
+        <f t="shared" si="6"/>
+        <v>"0","1","2","4",</v>
+      </c>
+      <c r="N5" t="s">
+        <v>228</v>
+      </c>
+      <c r="O5" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>"1 minute",</v>
+      </c>
+      <c r="P5" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>"0","1 round","5 round","1 minute",</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="7">
+        <v>1000</v>
+      </c>
+      <c r="C6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>"1,000",</v>
+      </c>
+      <c r="D6" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v>"0","1","10","100","1,000",</v>
+      </c>
+      <c r="E6" s="7">
+        <v>30</v>
+      </c>
+      <c r="F6" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>"30",</v>
+      </c>
+      <c r="G6" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>"0","1","3","10","30",</v>
+      </c>
+      <c r="K6" s="7">
+        <v>8</v>
+      </c>
+      <c r="L6" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>"8",</v>
+      </c>
+      <c r="M6" s="7" t="str">
+        <f t="shared" si="6"/>
+        <v>"0","1","2","4","8",</v>
+      </c>
+      <c r="N6" t="s">
+        <v>229</v>
+      </c>
+      <c r="O6" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>"10 minutes",</v>
+      </c>
+      <c r="P6" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>"0","1 round","5 round","1 minute","10 minutes",</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="7">
+        <v>10000</v>
+      </c>
+      <c r="C7" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>"10,000",</v>
+      </c>
+      <c r="D7" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v>"0","1","10","100","1,000","10,000",</v>
+      </c>
+      <c r="E7" s="7">
+        <v>100</v>
+      </c>
+      <c r="F7" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>"100",</v>
+      </c>
+      <c r="G7" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>"0","1","3","10","30","100",</v>
+      </c>
+      <c r="K7" s="7">
+        <v>15</v>
+      </c>
+      <c r="L7" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>"15",</v>
+      </c>
+      <c r="M7" s="7" t="str">
+        <f t="shared" si="6"/>
+        <v>"0","1","2","4","8","15",</v>
+      </c>
+      <c r="N7" t="s">
+        <v>230</v>
+      </c>
+      <c r="O7" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>"1 hour",</v>
+      </c>
+      <c r="P7" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>"0","1 round","5 round","1 minute","10 minutes","1 hour",</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="7">
+        <v>100000</v>
+      </c>
+      <c r="C8" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>"100,000",</v>
+      </c>
+      <c r="D8" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v>"0","1","10","100","1,000","10,000","100,000",</v>
+      </c>
+      <c r="E8" s="7">
+        <v>300</v>
+      </c>
+      <c r="F8" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>"300",</v>
+      </c>
+      <c r="G8" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>"0","1","3","10","30","100","300",</v>
+      </c>
+      <c r="K8" s="7">
+        <v>30</v>
+      </c>
+      <c r="L8" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>"30",</v>
+      </c>
+      <c r="M8" s="7" t="str">
+        <f t="shared" si="6"/>
+        <v>"0","1","2","4","8","15","30",</v>
+      </c>
+      <c r="N8" t="s">
+        <v>231</v>
+      </c>
+      <c r="O8" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>"4 hours",</v>
+      </c>
+      <c r="P8" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>"0","1 round","5 round","1 minute","10 minutes","1 hour","4 hours",</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="7">
+        <v>1000000</v>
+      </c>
+      <c r="C9" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>"1,000,000",</v>
+      </c>
+      <c r="D9" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v>"0","1","10","100","1,000","10,000","100,000","1,000,000",</v>
+      </c>
+      <c r="E9" s="7">
+        <v>1000</v>
+      </c>
+      <c r="F9" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>"1,000",</v>
+      </c>
+      <c r="G9" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>"0","1","3","10","30","100","300","1,000",</v>
+      </c>
+      <c r="K9" s="7">
+        <v>60</v>
+      </c>
+      <c r="L9" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>"60",</v>
+      </c>
+      <c r="M9" s="7" t="str">
+        <f t="shared" si="6"/>
+        <v>"0","1","2","4","8","15","30","60",</v>
+      </c>
+      <c r="N9" t="s">
+        <v>232</v>
+      </c>
+      <c r="O9" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>"12 hours",</v>
+      </c>
+      <c r="P9" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>"0","1 round","5 round","1 minute","10 minutes","1 hour","4 hours","12 hours",</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="7">
+        <v>10000000</v>
+      </c>
+      <c r="C10" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>"10,000,000",</v>
+      </c>
+      <c r="D10" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v>"0","1","10","100","1,000","10,000","100,000","1,000,000","10,000,000",</v>
+      </c>
+      <c r="E10" s="7">
+        <v>3000</v>
+      </c>
+      <c r="F10" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>"3,000",</v>
+      </c>
+      <c r="G10" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>"0","1","3","10","30","100","300","1,000","3,000",</v>
+      </c>
+      <c r="K10" s="7">
+        <v>125</v>
+      </c>
+      <c r="L10" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>"125",</v>
+      </c>
+      <c r="M10" s="7" t="str">
+        <f t="shared" si="6"/>
+        <v>"0","1","2","4","8","15","30","60","125",</v>
+      </c>
+      <c r="N10" t="s">
+        <v>233</v>
+      </c>
+      <c r="O10" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>"1 day",</v>
+      </c>
+      <c r="P10" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>"0","1 round","5 round","1 minute","10 minutes","1 hour","4 hours","12 hours","1 day",</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="7">
+        <v>100000000</v>
+      </c>
+      <c r="C11" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>"100,000,000",</v>
+      </c>
+      <c r="D11" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v>"0","1","10","100","1,000","10,000","100,000","1,000,000","10,000,000","100,000,000",</v>
+      </c>
+      <c r="E11" s="7">
+        <v>10000</v>
+      </c>
+      <c r="F11" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>"10,000",</v>
+      </c>
+      <c r="G11" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>"0","1","3","10","30","100","300","1,000","3,000","10,000",</v>
+      </c>
+      <c r="K11" s="7">
+        <v>250</v>
+      </c>
+      <c r="L11" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>"250",</v>
+      </c>
+      <c r="M11" s="7" t="str">
+        <f t="shared" si="6"/>
+        <v>"0","1","2","4","8","15","30","60","125","250",</v>
+      </c>
+      <c r="N11" t="s">
+        <v>234</v>
+      </c>
+      <c r="O11" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>"1 week",</v>
+      </c>
+      <c r="P11" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>"0","1 round","5 round","1 minute","10 minutes","1 hour","4 hours","12 hours","1 day","1 week",</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" s="7">
+        <v>1000000000</v>
+      </c>
+      <c r="C12" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>"1,000,000,000",</v>
+      </c>
+      <c r="D12" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v>"0","1","10","100","1,000","10,000","100,000","1,000,000","10,000,000","100,000,000","1,000,000,000",</v>
+      </c>
+      <c r="E12" s="7">
+        <v>30000</v>
+      </c>
+      <c r="F12" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>"30,000",</v>
+      </c>
+      <c r="G12" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>"0","1","3","10","30","100","300","1,000","3,000","10,000","30,000",</v>
+      </c>
+      <c r="K12" s="7">
+        <v>500</v>
+      </c>
+      <c r="L12" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>"500",</v>
+      </c>
+      <c r="M12" s="7" t="str">
+        <f t="shared" si="6"/>
+        <v>"0","1","2","4","8","15","30","60","125","250","500",</v>
+      </c>
+      <c r="N12" t="s">
+        <v>235</v>
+      </c>
+      <c r="O12" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>"1 month",</v>
+      </c>
+      <c r="P12" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>"0","1 round","5 round","1 minute","10 minutes","1 hour","4 hours","12 hours","1 day","1 week","1 month",</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" s="7">
+        <v>10000000000</v>
+      </c>
+      <c r="C13" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>"10,000,000,000",</v>
+      </c>
+      <c r="D13" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v>"0","1","10","100","1,000","10,000","100,000","1,000,000","10,000,000","100,000,000","1,000,000,000","10,000,000,000",</v>
+      </c>
+      <c r="E13" s="7">
+        <v>100000</v>
+      </c>
+      <c r="F13" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>"100,000",</v>
+      </c>
+      <c r="G13" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>"0","1","3","10","30","100","300","1,000","3,000","10,000","30,000","100,000",</v>
+      </c>
+      <c r="K13" s="7">
+        <v>1000</v>
+      </c>
+      <c r="L13" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>"1,000",</v>
+      </c>
+      <c r="M13" s="7" t="str">
+        <f t="shared" si="6"/>
+        <v>"0","1","2","4","8","15","30","60","125","250","500","1,000",</v>
+      </c>
+      <c r="N13" t="s">
+        <v>236</v>
+      </c>
+      <c r="O13" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>"1 season",</v>
+      </c>
+      <c r="P13" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>"0","1 round","5 round","1 minute","10 minutes","1 hour","4 hours","12 hours","1 day","1 week","1 month","1 season",</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" s="7">
+        <v>100000000000</v>
+      </c>
+      <c r="C14" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>"100,000,000,000",</v>
+      </c>
+      <c r="D14" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v>"0","1","10","100","1,000","10,000","100,000","1,000,000","10,000,000","100,000,000","1,000,000,000","10,000,000,000","100,000,000,000",</v>
+      </c>
+      <c r="E14" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F14" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>"300,000",</v>
+      </c>
+      <c r="G14" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>"0","1","3","10","30","100","300","1,000","3,000","10,000","30,000","100,000","300,000",</v>
+      </c>
+      <c r="K14" s="7">
+        <v>2000</v>
+      </c>
+      <c r="L14" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>"2,000",</v>
+      </c>
+      <c r="M14" s="7" t="str">
+        <f t="shared" si="6"/>
+        <v>"0","1","2","4","8","15","30","60","125","250","500","1,000","2,000",</v>
+      </c>
+      <c r="N14" t="s">
+        <v>237</v>
+      </c>
+      <c r="O14" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>"1 year",</v>
+      </c>
+      <c r="P14" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>"0","1 round","5 round","1 minute","10 minutes","1 hour","4 hours","12 hours","1 day","1 week","1 month","1 season","1 year",</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" s="7">
+        <v>1000000000000</v>
+      </c>
+      <c r="C15" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>"1,000,000,000,000",</v>
+      </c>
+      <c r="D15" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v>"0","1","10","100","1,000","10,000","100,000","1,000,000","10,000,000","100,000,000","1,000,000,000","10,000,000,000","100,000,000,000","1,000,000,000,000",</v>
+      </c>
+      <c r="E15" s="7">
+        <v>1000000</v>
+      </c>
+      <c r="F15" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>"1,000,000",</v>
+      </c>
+      <c r="G15" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>"0","1","3","10","30","100","300","1,000","3,000","10,000","30,000","100,000","300,000","1,000,000",</v>
+      </c>
+      <c r="K15" s="7">
+        <v>4000</v>
+      </c>
+      <c r="L15" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>"4,000",</v>
+      </c>
+      <c r="M15" s="7" t="str">
+        <f t="shared" si="6"/>
+        <v>"0","1","2","4","8","15","30","60","125","250","500","1,000","2,000","4,000",</v>
+      </c>
+      <c r="N15" t="s">
+        <v>238</v>
+      </c>
+      <c r="O15" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>"10 years",</v>
+      </c>
+      <c r="P15" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>"0","1 round","5 round","1 minute","10 minutes","1 hour","4 hours","12 hours","1 day","1 week","1 month","1 season","1 year","10 years",</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" s="7">
+        <v>10000000000000</v>
+      </c>
+      <c r="C16" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>"10,000,000,000,000",</v>
+      </c>
+      <c r="D16" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v>"0","1","10","100","1,000","10,000","100,000","1,000,000","10,000,000","100,000,000","1,000,000,000","10,000,000,000","100,000,000,000","1,000,000,000,000","10,000,000,000,000",</v>
+      </c>
+      <c r="E16" s="7">
+        <v>3000000</v>
+      </c>
+      <c r="F16" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>"3,000,000",</v>
+      </c>
+      <c r="G16" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>"0","1","3","10","30","100","300","1,000","3,000","10,000","30,000","100,000","300,000","1,000,000","3,000,000",</v>
+      </c>
+      <c r="K16" s="7">
+        <v>8000</v>
+      </c>
+      <c r="L16" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>"8,000",</v>
+      </c>
+      <c r="M16" s="7" t="str">
+        <f t="shared" si="6"/>
+        <v>"0","1","2","4","8","15","30","60","125","250","500","1,000","2,000","4,000","8,000",</v>
+      </c>
+      <c r="N16" t="s">
+        <v>239</v>
+      </c>
+      <c r="O16" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>"100 years",</v>
+      </c>
+      <c r="P16" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>"0","1 round","5 round","1 minute","10 minutes","1 hour","4 hours","12 hours","1 day","1 week","1 month","1 season","1 year","10 years","100 years",</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" s="7">
+        <v>100000000000000</v>
+      </c>
+      <c r="C17" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>"100,000,000,000,000",</v>
+      </c>
+      <c r="D17" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v>"0","1","10","100","1,000","10,000","100,000","1,000,000","10,000,000","100,000,000","1,000,000,000","10,000,000,000","100,000,000,000","1,000,000,000,000","10,000,000,000,000","100,000,000,000,000",</v>
+      </c>
+      <c r="E17" s="7">
+        <v>10000000</v>
+      </c>
+      <c r="F17" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>"10,000,000",</v>
+      </c>
+      <c r="G17" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>"0","1","3","10","30","100","300","1,000","3,000","10,000","30,000","100,000","300,000","1,000,000","3,000,000","10,000,000",</v>
+      </c>
+      <c r="K17" s="7">
+        <v>15000</v>
+      </c>
+      <c r="L17" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>"15,000",</v>
+      </c>
+      <c r="M17" s="7" t="str">
+        <f t="shared" si="6"/>
+        <v>"0","1","2","4","8","15","30","60","125","250","500","1,000","2,000","4,000","8,000","15,000",</v>
+      </c>
+      <c r="N17" t="s">
+        <v>240</v>
+      </c>
+      <c r="O17" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>"1000 years",</v>
+      </c>
+      <c r="P17" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>"0","1 round","5 round","1 minute","10 minutes","1 hour","4 hours","12 hours","1 day","1 week","1 month","1 season","1 year","10 years","100 years","1000 years",</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" s="7">
+        <v>1000000000000000</v>
+      </c>
+      <c r="C18" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>"1,000,000,000,000,000",</v>
+      </c>
+      <c r="D18" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v>"0","1","10","100","1,000","10,000","100,000","1,000,000","10,000,000","100,000,000","1,000,000,000","10,000,000,000","100,000,000,000","1,000,000,000,000","10,000,000,000,000","100,000,000,000,000","1,000,000,000,000,000",</v>
+      </c>
+      <c r="E18" s="7">
+        <v>100000000</v>
+      </c>
+      <c r="F18" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>"100,000,000",</v>
+      </c>
+      <c r="G18" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>"0","1","3","10","30","100","300","1,000","3,000","10,000","30,000","100,000","300,000","1,000,000","3,000,000","10,000,000","100,000,000",</v>
+      </c>
+      <c r="K18" s="7">
+        <v>30000</v>
+      </c>
+      <c r="L18" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>"30,000",</v>
+      </c>
+      <c r="M18" s="7" t="str">
+        <f t="shared" si="6"/>
+        <v>"0","1","2","4","8","15","30","60","125","250","500","1,000","2,000","4,000","8,000","15,000","30,000",</v>
+      </c>
+      <c r="N18" t="s">
+        <v>224</v>
+      </c>
+      <c r="O18" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>"Permanent",</v>
+      </c>
+      <c r="P18" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>"0","1 round","5 round","1 minute","10 minutes","1 hour","4 hours","12 hours","1 day","1 week","1 month","1 season","1 year","10 years","100 years","1000 years","Permanent",</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D20" s="7" t="s">
+        <v>241</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3A5E84E-83A9-4F40-9F8C-6691FBBEAA76}">
+  <dimension ref="A1:M48"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:13" ht="13" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="K1" s="1"/>
+      <c r="M1" s="1"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>218</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B2B2D97-4344-4CCF-99B2-474DA336E487}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>